<commit_message>
Added Advanced ExtentReport and fixed the StaleElement Exception
</commit_message>
<xml_diff>
--- a/src/main/java/resources/generateduuid.xlsx
+++ b/src/main/java/resources/generateduuid.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="748">
   <si>
     <t>Vehicle uuid</t>
   </si>
@@ -1519,6 +1519,756 @@
   </si>
   <si>
     <t>2018-11-18T12:53:17.946</t>
+  </si>
+  <si>
+    <t>17u145t781k4f4h0ytt8rdo03ph1phl9</t>
+  </si>
+  <si>
+    <t>2018-11-18T13:44:52.198</t>
+  </si>
+  <si>
+    <t>61k0re8et37823gsdod2kadx07f6183p</t>
+  </si>
+  <si>
+    <t>2018-11-18T13:45:21.541</t>
+  </si>
+  <si>
+    <t>nw1lpd99ordd1hst1w0fmuc98ueo6bs1</t>
+  </si>
+  <si>
+    <t>2018-11-18T13:46:23.893</t>
+  </si>
+  <si>
+    <t>g0ppkhet375tk5n9dr6yzwc06k727u3t</t>
+  </si>
+  <si>
+    <t>2018-11-18T13:47:19.423</t>
+  </si>
+  <si>
+    <t>1ck483036u27qy716uk27531porurj2v</t>
+  </si>
+  <si>
+    <t>2018-11-18T13:48:19.546</t>
+  </si>
+  <si>
+    <t>gb711nw27w17f171a3d12tz7g4t17les</t>
+  </si>
+  <si>
+    <t>2018-11-18T13:49:19.036</t>
+  </si>
+  <si>
+    <t>p9o1thjcg5jsevwucr5d92xfmv3oou64</t>
+  </si>
+  <si>
+    <t>2018-11-18T14:18:17.126</t>
+  </si>
+  <si>
+    <t>bv103ve3ib9z64b224ag2j1qqi6s1fh1</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:28:07.658</t>
+  </si>
+  <si>
+    <t>gp9015o381pi2mg0jxhx7cu476c3yp3k</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:31:35.670</t>
+  </si>
+  <si>
+    <t>muyc735buik6h13apf184q0p3k511y5j</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:32:20.710</t>
+  </si>
+  <si>
+    <t>8p287960cc7tebo1o02119d2rffct6xq</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:33:21.771</t>
+  </si>
+  <si>
+    <t>7s3o2t6w693sgvd5r0071573m0rm0tm0</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:34:22.426</t>
+  </si>
+  <si>
+    <t>icksbpws017y74le6pi462cuslw9km89</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:35:22.066</t>
+  </si>
+  <si>
+    <t>nwdm8tn8x71747ju8nvdb2pv1x3cgyfv</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:36:22.097</t>
+  </si>
+  <si>
+    <t>1m9p79q00z6xc30z7037110916401pc6</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:37:17.320</t>
+  </si>
+  <si>
+    <t>8099h0tpr7663rrqgbn5cu918bmmhv45</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:37:30.943</t>
+  </si>
+  <si>
+    <t>9of0uz0zx9750a58rzywblg8725m5c38</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:37:46.403</t>
+  </si>
+  <si>
+    <t>k6u21iuy23xs5m6hv542dtr9cujbf9r6</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:38:26.024</t>
+  </si>
+  <si>
+    <t>83c2rmuhmaeb915wump31ynema827s7s</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:39:21.642</t>
+  </si>
+  <si>
+    <t>a6sxn817g34630o5e51w17i4zqdhxhti</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:40:24.605</t>
+  </si>
+  <si>
+    <t>346r60m4w7dvcnwow693u145r92b2e98</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:41:21.638</t>
+  </si>
+  <si>
+    <t>vu0v66i6p8pv523b03psv5295r4ze598</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:41:35.639</t>
+  </si>
+  <si>
+    <t>758u354udtp8tm8kytg3awg2ef1l2wd5</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:41:50.058</t>
+  </si>
+  <si>
+    <t>olzrb7m58kzx58xuzy1k5i9f8q5714d5</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:42:04.346</t>
+  </si>
+  <si>
+    <t>bh301ehyxb0m4m9q7130e125fp1p86pr</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:45:04.989</t>
+  </si>
+  <si>
+    <t>b5n3vv7y1am9sk0qyi5eg8plhn2981l6</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:46:20.346</t>
+  </si>
+  <si>
+    <t>9a4i6tbafg7f64mw0fe95fprv6k7bvi4</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:47:21.474</t>
+  </si>
+  <si>
+    <t>434swwn50350ufy339vrca6w575a5ojs</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:48:22.572</t>
+  </si>
+  <si>
+    <t>l1hhystxc341gj2tp26rjhb7for47he2</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:49:24.688</t>
+  </si>
+  <si>
+    <t>wk5n2c5f5bo1guqqp0942u59srw7n08l</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:50:19.727</t>
+  </si>
+  <si>
+    <t>tzz28fi28stv5h1t58pcmcs79i85k91d</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:51:19.734</t>
+  </si>
+  <si>
+    <t>164z658pale6u6chvx9wh1oc9wy68evi</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:51:32.663</t>
+  </si>
+  <si>
+    <t>f4rsh79h5uj3hh58i74ivrvm020fupx3</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:51:45.771</t>
+  </si>
+  <si>
+    <t>jz8t65n972od3vk6t528f7cduf5os62l</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:52:20.572</t>
+  </si>
+  <si>
+    <t>4e8n4t09945a806the6470q33h040856</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:53:21.043</t>
+  </si>
+  <si>
+    <t>3bvn1zi4ff1gtigse438mt0641ue0pqx</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:54:20.889</t>
+  </si>
+  <si>
+    <t>iy7l018iqcuewvw7htzqphmq0d2nbdb2</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:54:35.176</t>
+  </si>
+  <si>
+    <t>4a6j74zzsg3l9670a5hg4x9tas939a2n</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:54:49.729</t>
+  </si>
+  <si>
+    <t>w7di2onaj13jg59m0vyagyls5ie90ep8</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:55:04.112</t>
+  </si>
+  <si>
+    <t>yu9ivh0tzfkp32gi510njw6vducgxat3</t>
+  </si>
+  <si>
+    <t>2018-11-18T15:55:18.340</t>
+  </si>
+  <si>
+    <t>s0cgc244hzej8lbqhau08hur3u6q81is</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:02:35.231</t>
+  </si>
+  <si>
+    <t>hi67x26zandpj3w06yu0kb27g3c07057</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:03:22.739</t>
+  </si>
+  <si>
+    <t>3t94q6n1ozmd43ly3fl391tyx0zp45ov</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:04:22.800</t>
+  </si>
+  <si>
+    <t>0cc4bp76ubqd0y7lq47d3e71ze0t0c0v</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:05:23.926</t>
+  </si>
+  <si>
+    <t>uxjk5j0b13tr2aa9n91s9o7d0xo7p9e2</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:06:20.929</t>
+  </si>
+  <si>
+    <t>yrvtns4ui6v57iac45ri9rkh4vu934df</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:07:22.010</t>
+  </si>
+  <si>
+    <t>x333aez1xm8r3pvs3tcs2xcod0g2azt5</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:08:23.681</t>
+  </si>
+  <si>
+    <t>5a589dg78il0i3kd0bze3cm9znwx7o08</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:08:37.954</t>
+  </si>
+  <si>
+    <t>tdlv76kneitdzvm64862738j2b02fo80</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:08:52.212</t>
+  </si>
+  <si>
+    <t>rl8tr2jy131z6fhuo4706dkj95mhn40y</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:09:22.954</t>
+  </si>
+  <si>
+    <t>qpmj84y0614yc3q0viqsb6dg6u1ab64u</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:10:18.199</t>
+  </si>
+  <si>
+    <t>91o07d89tq9q4m0t9vq5a6urxi7936bu</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:10:32.357</t>
+  </si>
+  <si>
+    <t>vnl890oox3eqi0pm6bn48y4f1y129400</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:11:24.729</t>
+  </si>
+  <si>
+    <t>y0yzyx1q2j02tml92ex6y6705g1j7t79</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:11:55.075</t>
+  </si>
+  <si>
+    <t>dj2uu5l3sd692g38rndxatvb6xjtf50z</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:12:22.458</t>
+  </si>
+  <si>
+    <t>exzq6dvztg0eudi2p1zrd6m2zo845f72</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:13:20.658</t>
+  </si>
+  <si>
+    <t>2k901zc80n00ys5p87dx8890pxogodcn</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:14:22.307</t>
+  </si>
+  <si>
+    <t>17v67h37j4r3wy8tc1bb3vuj2g53geqv</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:14:37.106</t>
+  </si>
+  <si>
+    <t>po05wk2b0570ez28wf25srd2bt675fl8</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:14:51.823</t>
+  </si>
+  <si>
+    <t>c802tu5xdix0dqjq0cs7qxix4z016wj1</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:15:06.690</t>
+  </si>
+  <si>
+    <t>52yf6xzc64nqv6386lotkkt0jwr91z0h</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:32:33.982</t>
+  </si>
+  <si>
+    <t>ak9toi8uuh4t02b170ap7rh282p3n5g2</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:33:20.646</t>
+  </si>
+  <si>
+    <t>n23ay9drpo68zi6krh822n87ge2ytf4f</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:34:23.268</t>
+  </si>
+  <si>
+    <t>23dc3bbd2hiu1kz0o8f68efwai0v2nhu</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:35:19.363</t>
+  </si>
+  <si>
+    <t>rpnrv13rxfg87yhjqd49ilvi76ziywlj</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:36:14.683</t>
+  </si>
+  <si>
+    <t>18m8befl84wu6uuk5816c8xdie8gy822</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:37:26.135</t>
+  </si>
+  <si>
+    <t>lary9ua94f15c56g0x7hy7a7573796eq</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:38:19.683</t>
+  </si>
+  <si>
+    <t>y5st0w25khqx1pa8ixp7uw1gmjy81kk3</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:38:33.770</t>
+  </si>
+  <si>
+    <t>b53z3rxlpx39723b0rd7tt4v0g8yz829</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:38:48.868</t>
+  </si>
+  <si>
+    <t>zqny38a93g27rtx2hloqv581v1qs22mi</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:39:20.596</t>
+  </si>
+  <si>
+    <t>4qb833ft0491c3056i4sqbl0u95r781l</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:40:23.414</t>
+  </si>
+  <si>
+    <t>36sjmwe01ob9m24q2dfsi646y8x1c84m</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:41:21.065</t>
+  </si>
+  <si>
+    <t>c4n8y556akax7xqh2bd38896ayzogt9h</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:42:25.294</t>
+  </si>
+  <si>
+    <t>8592f723be79f9dxal85ua9w7w3jni35</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:43:25.448</t>
+  </si>
+  <si>
+    <t>tzanx756wvzmbi5j044s0th8725byfm2</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:44:23.533</t>
+  </si>
+  <si>
+    <t>o2yy3d563xey80391qb0xqn2dsngvbyk</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:45:20.351</t>
+  </si>
+  <si>
+    <t>7mriqgv4hg7ns0gzz83p16e6ud21zyrs</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:46:21.303</t>
+  </si>
+  <si>
+    <t>51kdnu2q13k34jzi0s6n277xz3iq9891</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:46:38.040</t>
+  </si>
+  <si>
+    <t>m0hn7ve7f21y02dm5x2lbmbms9dbgjv0</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:46:53.091</t>
+  </si>
+  <si>
+    <t>my8fun79j02u78rgbz07l7xw03sq954n</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:47:08.564</t>
+  </si>
+  <si>
+    <t>nk5og5jnwx8hfth8on389axo077lb84w</t>
+  </si>
+  <si>
+    <t>2018-11-18T16:57:03.971</t>
+  </si>
+  <si>
+    <t>ul9176ls41ajvilt54r21o88n9p54p6s</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:03:27.886</t>
+  </si>
+  <si>
+    <t>570818mbvhbm73kjmu01qfm8p1nlmg5r</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:03:42.806</t>
+  </si>
+  <si>
+    <t>t6eh2114my1pv22lg5bvc329c3gdww82</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:03:58.183</t>
+  </si>
+  <si>
+    <t>4qsd9u5ooi9032v5wh6260hd9l83bo77</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:04:16.619</t>
+  </si>
+  <si>
+    <t>o3ku82mui3otkkl32xgep3vuz4eom9pb</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:04:32.519</t>
+  </si>
+  <si>
+    <t>om2z9n0g2w31po4kj32g94v8b9aig4pj</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:04:49.365</t>
+  </si>
+  <si>
+    <t>83weialxk16tll24y4jy9bw0f2669wwe</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:05:05.208</t>
+  </si>
+  <si>
+    <t>w97864c0k18017210d70s08fq4luxk95</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:05:22.504</t>
+  </si>
+  <si>
+    <t>vm87d8t22m5sn6e4f80jl2pi62j7hvo9</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:05:37.939</t>
+  </si>
+  <si>
+    <t>24zqime6crdwm99dc2gc69zy6tjpuosw</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:05:54.402</t>
+  </si>
+  <si>
+    <t>lg63s7ngi9pjfo732v5h0h6v4i0slmyi</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:06:10.410</t>
+  </si>
+  <si>
+    <t>qdtn77qpv9cfy8hmq7du2k84t6ssmhtj</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:06:27.449</t>
+  </si>
+  <si>
+    <t>w5bfw15xd4258vr2159ll42g382p918a</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:06:44.850</t>
+  </si>
+  <si>
+    <t>x936a1f6xjvda8hdw5j6fd2ft3t153w6</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:07:04.817</t>
+  </si>
+  <si>
+    <t>5i66067brcglbm5nfrv0c59s08s35sq0</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:07:19.979</t>
+  </si>
+  <si>
+    <t>ua709uib7z6z69hwd14dkmo1o29js64j</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:07:39.878</t>
+  </si>
+  <si>
+    <t>84lhgbwghk8mjb5ivmw4h4va2zzs5n75</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:07:59.141</t>
+  </si>
+  <si>
+    <t>p56f4vv7tm7532va85zl873r3p4adp08</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:08:19.990</t>
+  </si>
+  <si>
+    <t>5o5w8e5eo0o8z9a5ux57g2vx17ki3298</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:08:40.397</t>
+  </si>
+  <si>
+    <t>aelc492u53etxfo2oiq8zq5bc1mnkf69</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:08:58.718</t>
+  </si>
+  <si>
+    <t>d5f6d9m392i5th4i8i642a592p8o7e65</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:14:00.682</t>
+  </si>
+  <si>
+    <t>ft320y7g3u85qb8lizu4el90kdxzf4ay</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:14:21.451</t>
+  </si>
+  <si>
+    <t>1jf7jsfuvadhoky84fonzq147z58419x</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:15:24.255</t>
+  </si>
+  <si>
+    <t>vwj9tz7d30i9gd73na0taylkmflj40e3</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:16:20.564</t>
+  </si>
+  <si>
+    <t>9c9506c6k5klhk58a5w62p7ch34uveje</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:17:22.364</t>
+  </si>
+  <si>
+    <t>tmaf9i38q53e71g3vn3y2j8z4rfp5448</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:18:27.485</t>
+  </si>
+  <si>
+    <t>bd1753tkfh8yn2llgah9fr8yq303grj2</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:19:23.895</t>
+  </si>
+  <si>
+    <t>g9131e6oyl4tb5udb7vku7apr0b5ev0l</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:19:38.387</t>
+  </si>
+  <si>
+    <t>zr4c308d419hhug1lu488a0pp0135u9n</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:19:52.727</t>
+  </si>
+  <si>
+    <t>g2klp2g63h2o0fyust87tnqer962ha98</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:20:19.223</t>
+  </si>
+  <si>
+    <t>alzulzv5x3jkgiqcjjrs38qfn9a2r10f</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:21:24.948</t>
+  </si>
+  <si>
+    <t>ya1e8j516sxux5a159mqvjrq5rsffl4e</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:22:25.715</t>
+  </si>
+  <si>
+    <t>kynt14ns11b8ovvyz5lzcxv7oe8f19m5</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:24:56.217</t>
+  </si>
+  <si>
+    <t>8r4o2qwdikbhgjc8g3t524e8ihhg0nt5</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:25:17.850</t>
+  </si>
+  <si>
+    <t>sp0tbe18720cdz41d30sjsmayc9x72pd</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:26:18.612</t>
+  </si>
+  <si>
+    <t>57v9um019g316s170orbmc7t5jd028w8</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:27:23.880</t>
+  </si>
+  <si>
+    <t>10dp7q74fbm6qmtsu8mawe208yh3m6t8</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:28:23.629</t>
+  </si>
+  <si>
+    <t>tfuyiktzdz33j4u2fz3h9g9ugw1dxm98</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:28:39.937</t>
+  </si>
+  <si>
+    <t>95xq8rgxb12j200s5u5py603c2e2460x</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:28:54.806</t>
+  </si>
+  <si>
+    <t>6o21hu35gf931munpncl662lql8c9fq5</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:29:09.787</t>
+  </si>
+  <si>
+    <t>jfi8n0r513yk0ib724alt2hhff351699</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:30:44.332</t>
+  </si>
+  <si>
+    <t>50h741465o4q0mp3el9f1u713a94x09m</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:30:58.118</t>
+  </si>
+  <si>
+    <t>oe9g01ylr09455e9162w047j7534zvb5</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:31:26.736</t>
+  </si>
+  <si>
+    <t>75nngn8ucoqhb3nxtgq25wiay5ths7c7</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:32:18.941</t>
   </si>
 </sst>
 </file>
@@ -3874,6 +4624,1006 @@
         <v>497</v>
       </c>
     </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>498</v>
+      </c>
+      <c r="B251" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>500</v>
+      </c>
+      <c r="B252" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>502</v>
+      </c>
+      <c r="B253" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>504</v>
+      </c>
+      <c r="B254" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>506</v>
+      </c>
+      <c r="B255" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>508</v>
+      </c>
+      <c r="B256" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>510</v>
+      </c>
+      <c r="B257" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>512</v>
+      </c>
+      <c r="B258" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>514</v>
+      </c>
+      <c r="B259" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>516</v>
+      </c>
+      <c r="B260" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>518</v>
+      </c>
+      <c r="B261" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>520</v>
+      </c>
+      <c r="B262" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>522</v>
+      </c>
+      <c r="B263" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>524</v>
+      </c>
+      <c r="B264" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>526</v>
+      </c>
+      <c r="B265" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>528</v>
+      </c>
+      <c r="B266" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>530</v>
+      </c>
+      <c r="B267" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>532</v>
+      </c>
+      <c r="B268" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>534</v>
+      </c>
+      <c r="B269" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>536</v>
+      </c>
+      <c r="B270" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>538</v>
+      </c>
+      <c r="B271" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>540</v>
+      </c>
+      <c r="B272" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>542</v>
+      </c>
+      <c r="B273" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>544</v>
+      </c>
+      <c r="B274" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>546</v>
+      </c>
+      <c r="B275" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>548</v>
+      </c>
+      <c r="B276" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>550</v>
+      </c>
+      <c r="B277" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>552</v>
+      </c>
+      <c r="B278" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>554</v>
+      </c>
+      <c r="B279" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>556</v>
+      </c>
+      <c r="B280" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>558</v>
+      </c>
+      <c r="B281" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>560</v>
+      </c>
+      <c r="B282" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>562</v>
+      </c>
+      <c r="B283" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>564</v>
+      </c>
+      <c r="B284" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>566</v>
+      </c>
+      <c r="B285" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>568</v>
+      </c>
+      <c r="B286" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>570</v>
+      </c>
+      <c r="B287" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>572</v>
+      </c>
+      <c r="B288" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>574</v>
+      </c>
+      <c r="B289" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>576</v>
+      </c>
+      <c r="B290" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>578</v>
+      </c>
+      <c r="B291" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>580</v>
+      </c>
+      <c r="B292" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>582</v>
+      </c>
+      <c r="B293" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>584</v>
+      </c>
+      <c r="B294" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>586</v>
+      </c>
+      <c r="B295" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>588</v>
+      </c>
+      <c r="B296" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>590</v>
+      </c>
+      <c r="B297" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>592</v>
+      </c>
+      <c r="B298" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>594</v>
+      </c>
+      <c r="B299" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>596</v>
+      </c>
+      <c r="B300" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>598</v>
+      </c>
+      <c r="B301" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>600</v>
+      </c>
+      <c r="B302" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>602</v>
+      </c>
+      <c r="B303" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>604</v>
+      </c>
+      <c r="B304" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>606</v>
+      </c>
+      <c r="B305" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>608</v>
+      </c>
+      <c r="B306" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>610</v>
+      </c>
+      <c r="B307" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>612</v>
+      </c>
+      <c r="B308" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>614</v>
+      </c>
+      <c r="B309" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>616</v>
+      </c>
+      <c r="B310" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>618</v>
+      </c>
+      <c r="B311" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>620</v>
+      </c>
+      <c r="B312" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>622</v>
+      </c>
+      <c r="B313" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>624</v>
+      </c>
+      <c r="B314" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>626</v>
+      </c>
+      <c r="B315" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>628</v>
+      </c>
+      <c r="B316" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>630</v>
+      </c>
+      <c r="B317" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>632</v>
+      </c>
+      <c r="B318" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>634</v>
+      </c>
+      <c r="B319" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>636</v>
+      </c>
+      <c r="B320" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>638</v>
+      </c>
+      <c r="B321" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>640</v>
+      </c>
+      <c r="B322" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>642</v>
+      </c>
+      <c r="B323" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>644</v>
+      </c>
+      <c r="B324" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>646</v>
+      </c>
+      <c r="B325" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>648</v>
+      </c>
+      <c r="B326" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>650</v>
+      </c>
+      <c r="B327" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>652</v>
+      </c>
+      <c r="B328" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>654</v>
+      </c>
+      <c r="B329" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>656</v>
+      </c>
+      <c r="B330" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>658</v>
+      </c>
+      <c r="B331" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>660</v>
+      </c>
+      <c r="B332" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>662</v>
+      </c>
+      <c r="B333" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>664</v>
+      </c>
+      <c r="B334" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>666</v>
+      </c>
+      <c r="B335" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>668</v>
+      </c>
+      <c r="B336" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>670</v>
+      </c>
+      <c r="B337" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>672</v>
+      </c>
+      <c r="B338" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>674</v>
+      </c>
+      <c r="B339" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>676</v>
+      </c>
+      <c r="B340" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>678</v>
+      </c>
+      <c r="B341" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>680</v>
+      </c>
+      <c r="B342" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>682</v>
+      </c>
+      <c r="B343" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>684</v>
+      </c>
+      <c r="B344" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>686</v>
+      </c>
+      <c r="B345" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>688</v>
+      </c>
+      <c r="B346" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>690</v>
+      </c>
+      <c r="B347" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>692</v>
+      </c>
+      <c r="B348" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>694</v>
+      </c>
+      <c r="B349" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>696</v>
+      </c>
+      <c r="B350" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>698</v>
+      </c>
+      <c r="B351" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>700</v>
+      </c>
+      <c r="B352" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s">
+        <v>702</v>
+      </c>
+      <c r="B353" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s">
+        <v>704</v>
+      </c>
+      <c r="B354" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s">
+        <v>706</v>
+      </c>
+      <c r="B355" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s">
+        <v>708</v>
+      </c>
+      <c r="B356" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s">
+        <v>710</v>
+      </c>
+      <c r="B357" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s">
+        <v>712</v>
+      </c>
+      <c r="B358" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s">
+        <v>714</v>
+      </c>
+      <c r="B359" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s">
+        <v>716</v>
+      </c>
+      <c r="B360" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s">
+        <v>718</v>
+      </c>
+      <c r="B361" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s">
+        <v>720</v>
+      </c>
+      <c r="B362" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s">
+        <v>722</v>
+      </c>
+      <c r="B363" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s">
+        <v>724</v>
+      </c>
+      <c r="B364" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s">
+        <v>726</v>
+      </c>
+      <c r="B365" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s">
+        <v>728</v>
+      </c>
+      <c r="B366" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s">
+        <v>730</v>
+      </c>
+      <c r="B367" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s">
+        <v>732</v>
+      </c>
+      <c r="B368" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s">
+        <v>734</v>
+      </c>
+      <c r="B369" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s">
+        <v>736</v>
+      </c>
+      <c r="B370" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s">
+        <v>738</v>
+      </c>
+      <c r="B371" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s">
+        <v>740</v>
+      </c>
+      <c r="B372" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s">
+        <v>742</v>
+      </c>
+      <c r="B373" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s">
+        <v>744</v>
+      </c>
+      <c r="B374" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="s">
+        <v>746</v>
+      </c>
+      <c r="B375" t="s">
+        <v>747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing some bugs in the code, adding remove=true feature for the new vehicles
</commit_message>
<xml_diff>
--- a/src/main/java/resources/generateduuid.xlsx
+++ b/src/main/java/resources/generateduuid.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="1218">
   <si>
     <t>Vehicle uuid</t>
   </si>
@@ -2269,6 +2269,1416 @@
   </si>
   <si>
     <t>2018-11-18T17:32:18.941</t>
+  </si>
+  <si>
+    <t>509eh3218k46se5332u12t9t39f0upj5</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:34:59.576</t>
+  </si>
+  <si>
+    <t>ye9q7tt0zt6ebw0uzqk73k72695y8fsc</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:35:22.301</t>
+  </si>
+  <si>
+    <t>1231pof6rwz437p6jx93nf3heijln24a</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:36:23.482</t>
+  </si>
+  <si>
+    <t>r0c12xlo32p30ok3se97tj2308d6zpgu</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:37:24.456</t>
+  </si>
+  <si>
+    <t>tpqct68beiit9652y50c1317ng29u7lq</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:38:20.735</t>
+  </si>
+  <si>
+    <t>563qf6695o3rf8rwqaw3709kj4p1e86p</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:39:26.751</t>
+  </si>
+  <si>
+    <t>zv4g3t1k288nowy7ozd987p53410393l</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:40:20.312</t>
+  </si>
+  <si>
+    <t>zbgchnq89jc2am066kl16481e0d8w0r3</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:40:34.894</t>
+  </si>
+  <si>
+    <t>8c84bajkv90c1f1vcqo27d2q62aogm66</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:40:50.289</t>
+  </si>
+  <si>
+    <t>1ytnd265h14wf0h1h21mj5stt6r47h08</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:41:23.369</t>
+  </si>
+  <si>
+    <t>0isu4ft5dqk993v97ne26032wcrn9sb6</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:42:18.901</t>
+  </si>
+  <si>
+    <t>8ujkjc58f9lz69l569jqbrfkt7kk2f7r</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:43:19.920</t>
+  </si>
+  <si>
+    <t>04bf3952w1q7f6q5vx3271ks1380c7iw</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:44:21.094</t>
+  </si>
+  <si>
+    <t>8f3l0h50xz7s4mc3bs2zom946npfgb9r</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:45:18.823</t>
+  </si>
+  <si>
+    <t>tt4731f0j3eo5w0qre4fvbkkg5i96lc3</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:46:21.959</t>
+  </si>
+  <si>
+    <t>ya4rp9howteyd084t21zsu10jw6bv5y8</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:47:22.642</t>
+  </si>
+  <si>
+    <t>wx3k61c953pjiy3od3lc7xx4g15cak53</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:48:23.725</t>
+  </si>
+  <si>
+    <t>4k8731g8dquxi1px3yjkm231u5f8i15m</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:48:40.721</t>
+  </si>
+  <si>
+    <t>fq9me8ht51elp95te7sf2ukrxo48cf2j</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:48:57.773</t>
+  </si>
+  <si>
+    <t>y32qk5mo11eevptpx3rj5bo2piw0lkye</t>
+  </si>
+  <si>
+    <t>2018-11-18T17:49:13.921</t>
+  </si>
+  <si>
+    <t>0ciurfwgpmj49w4n97bzgd64ibq265w1</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:47:55.698</t>
+  </si>
+  <si>
+    <t>6l7hoxjsya7ap86ug408exnph29p0h6k</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:48:27.102</t>
+  </si>
+  <si>
+    <t>uv5d67yqhox8k6w4tq38kglk7ef5g8yo</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:49:23.452</t>
+  </si>
+  <si>
+    <t>2gz9k51bex5etsx99l367787uikpfkj2</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:50:24.388</t>
+  </si>
+  <si>
+    <t>cajj1y9g45b83kyhfqc6q79g80nl2lz9</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:53:15.412</t>
+  </si>
+  <si>
+    <t>ev0blj2532c6h4561o2b2s3b7zfble9l</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:54:22.116</t>
+  </si>
+  <si>
+    <t>oa947f615tdcz45qt5g8dl7k5e2xjhir</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:55:25.916</t>
+  </si>
+  <si>
+    <t>15aps426n6z401709agfc4tw7fbu9fk8</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:55:44.787</t>
+  </si>
+  <si>
+    <t>32urc82c8jons3gu9aq7v5846h97kvno</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:55:59.794</t>
+  </si>
+  <si>
+    <t>thlh54wusr1lial4fbrb039y0a12gtl9</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:56:21.491</t>
+  </si>
+  <si>
+    <t>h5us4ah6xwiq293thp02937lzd8b31c3</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:57:23.127</t>
+  </si>
+  <si>
+    <t>6on1v8q4lvq4vql8d8pqk9m8s6t87af2</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:58:19.590</t>
+  </si>
+  <si>
+    <t>y2n575bd333c8x15c286sh5uu8hy6748</t>
+  </si>
+  <si>
+    <t>2018-11-18T20:59:26.148</t>
+  </si>
+  <si>
+    <t>zf28y5b69j48vu02e4udwghq4oo9pr94</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:00:24.600</t>
+  </si>
+  <si>
+    <t>ee3etlsys3kk4wf417h8im6fr8189473</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:01:20.957</t>
+  </si>
+  <si>
+    <t>kb754y85gl9ncbr40jfevaa944ex9l2j</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:02:20.988</t>
+  </si>
+  <si>
+    <t>0c9y58fu5wu126su1ui6wunvi69m0b56</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:03:22.457</t>
+  </si>
+  <si>
+    <t>5sde8w0lgb5mv92jw3vv2nk3nt92kdjt</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:03:42.373</t>
+  </si>
+  <si>
+    <t>j0nac98027zjmwg45f71uutk0q917996</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:03:58.497</t>
+  </si>
+  <si>
+    <t>9m4cpgosequ36bw4347j0lbt7y00d97v</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:04:18.473</t>
+  </si>
+  <si>
+    <t>j4366afdvrfg68r2vpjnp8zvdnr3jj1p</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:15:53.908</t>
+  </si>
+  <si>
+    <t>axacp3hrwlth24898d1rb71v4d5ig16y</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:16:25.157</t>
+  </si>
+  <si>
+    <t>jkhbcp1c4kb78e1k12zl450xw8uib55i</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:20:43.875</t>
+  </si>
+  <si>
+    <t>95cho9v804ey5p3qxm4c5g04144v8w8v</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:21:19.751</t>
+  </si>
+  <si>
+    <t>101g9480cgqiq27ov6ytd8t67v2ztco7</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:22:21.817</t>
+  </si>
+  <si>
+    <t>bd9jms1i1iy36pyrx60kq6asset69xgd</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:24:59.189</t>
+  </si>
+  <si>
+    <t>5d6w1rhi81q197742781i1i7melh9te1</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:25:23.008</t>
+  </si>
+  <si>
+    <t>3h658j3gtim480yyryuszpe15e16sxs1</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:25:42.490</t>
+  </si>
+  <si>
+    <t>a2lh6lbc3sb5oh85a4400a6m0ahf47lv</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:26:20.454</t>
+  </si>
+  <si>
+    <t>a79d29m16w8d3e2lsnpme5048y3o99u6</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:27:20.925</t>
+  </si>
+  <si>
+    <t>f05rhz0xck820b831zhbm0h9pw1wf268</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:28:19.091</t>
+  </si>
+  <si>
+    <t>bfds338xnp36po4245cfyht442up9j97</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:29:23.817</t>
+  </si>
+  <si>
+    <t>2pv1nme0yipn88i8p94o4ma7l7in6y99</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:29:42.833</t>
+  </si>
+  <si>
+    <t>jy6zqihrre47jflhp13y6mek17tv3sdd</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:30:01.046</t>
+  </si>
+  <si>
+    <t>6h1fv1dzvzc21ibz8z782ytmie0ykdv1</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:33:48.127</t>
+  </si>
+  <si>
+    <t>ny0zidfc1i2h4g2m3wr1zg8ygq0lu4r9</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:34:18.486</t>
+  </si>
+  <si>
+    <t>0o77whst86vq4h97wm329ft9x94bxwhv</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:34:37.810</t>
+  </si>
+  <si>
+    <t>sqrv25s5bp1z9u6u9xy1epqsrznf2q2o</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:46:50.865</t>
+  </si>
+  <si>
+    <t>668fv9fsv6x3azhso38241273v6n0q5y</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:47:24.990</t>
+  </si>
+  <si>
+    <t>lml4si060iw3g6xuthoxl518ajt55v22</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:48:21.921</t>
+  </si>
+  <si>
+    <t>9f857ye4nws80udfu5h26gcmx1u7s3he</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:49:24.866</t>
+  </si>
+  <si>
+    <t>x6hax8407i9hh8le41unoq2e18njm42i</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:50:19.631</t>
+  </si>
+  <si>
+    <t>aztqwwhs9mf8q39ym0ey9q0qe557j68r</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:51:24.161</t>
+  </si>
+  <si>
+    <t>jo1v7fai400js240e6zyz0ed6ryvx9vy</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:52:23.841</t>
+  </si>
+  <si>
+    <t>wh2a0ajq4228j9edjcdy194i1crr17k6</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:52:42.871</t>
+  </si>
+  <si>
+    <t>ehq489k1nq5124ryh15flizm2y1a7429</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:53:01.719</t>
+  </si>
+  <si>
+    <t>7rn1xo19igu44g71h1s3ci312pi4k17f</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:57:26.270</t>
+  </si>
+  <si>
+    <t>olxeqa62kk4o67o92sn3h231wg7a80jt</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:58:19.707</t>
+  </si>
+  <si>
+    <t>v56q1sk0mvv7gdq37q5dr334w3kct9zj</t>
+  </si>
+  <si>
+    <t>2018-11-18T21:58:39.913</t>
+  </si>
+  <si>
+    <t>rx434sdg3snzsti84183c4rm8n278ql3</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:05:44.517</t>
+  </si>
+  <si>
+    <t>vbb6z70prg4c762azshmz0sx5zjdq579</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:06:02.943</t>
+  </si>
+  <si>
+    <t>237jvn8349s5olb522mhk8yrjd0ime91</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:10:02.823</t>
+  </si>
+  <si>
+    <t>zdm2ee6yxin732wnma1va23u9907gbat</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:11:26.927</t>
+  </si>
+  <si>
+    <t>1paa03tun2pu6g3x82pcp0c9xup3534u</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:12:20.043</t>
+  </si>
+  <si>
+    <t>pm6mta7ek393tfb83r30p45o65rih3my</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:13:18.748</t>
+  </si>
+  <si>
+    <t>c95o7t6jnzce9644oin28tq41h071dtc</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:14:24.930</t>
+  </si>
+  <si>
+    <t>5zf9sp8sl5qef26zj0d0391tywh3f4u0</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:14:44.629</t>
+  </si>
+  <si>
+    <t>89h9gt0qc26emzr5y2d8ph3tn6c36148</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:15:04.424</t>
+  </si>
+  <si>
+    <t>3quzjbceagxgz7itibj7pxjz95d584ex</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:16:25.988</t>
+  </si>
+  <si>
+    <t>1ssnd6g88c35foxrfb0ievs316ko0u93</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:17:26.858</t>
+  </si>
+  <si>
+    <t>dzts8460my4tiyij5i508x0d2300rsj9</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:17:46.893</t>
+  </si>
+  <si>
+    <t>2479tehmdy2451mrc19nk77rl138ej1p</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:31:01.936</t>
+  </si>
+  <si>
+    <t>v2wbjnhkmwc01aq5b83b4rb1t29n2w9l</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:33:27.072</t>
+  </si>
+  <si>
+    <t>rs59lz76hk22w008k716ylhaa4gf1a44</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:34:28.181</t>
+  </si>
+  <si>
+    <t>483gtbvof0h7xkp20ra2w5342ledgqos</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:35:27.189</t>
+  </si>
+  <si>
+    <t>18wdt82fs6ut495xy635xgq8ug6xg64q</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:36:25.543</t>
+  </si>
+  <si>
+    <t>3f21ts44lq7csz5g30e17xu17rn8z6er</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:37:23.490</t>
+  </si>
+  <si>
+    <t>6n0ja62k0p96s3zxcdhw23wg06uw71uh</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:38:21.949</t>
+  </si>
+  <si>
+    <t>k44batt155rl550qd70mzhdjh7x793i4</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:38:41.538</t>
+  </si>
+  <si>
+    <t>2040sufre0s7399o78t2p5l05u3i39u4</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:39:01.318</t>
+  </si>
+  <si>
+    <t>1vrx9hkj6qz618e0zw9mq8ixcov43q33</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:43:41.551</t>
+  </si>
+  <si>
+    <t>ol592vnfo2ic44oc0o1aajrm3v94agw5</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:44:27.435</t>
+  </si>
+  <si>
+    <t>92n5fateb3cf875875godrmc2131h1qf</t>
+  </si>
+  <si>
+    <t>2018-11-18T22:44:48.243</t>
+  </si>
+  <si>
+    <t>b0bx3o1rmr5fa9pjrc7qnxtq8coq812n</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:05:30.981</t>
+  </si>
+  <si>
+    <t>064tg857ornofh8f00v5oh1odv3bfaby</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:05:54.596</t>
+  </si>
+  <si>
+    <t>2h66hdf94v2dpde9d351ltq3ko7kg6a1</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:06:25.168</t>
+  </si>
+  <si>
+    <t>vpv3mjocc4dbz7cu6v0s8am8k35rgmwo</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:07:21.538</t>
+  </si>
+  <si>
+    <t>in8et961808pv5x67094ws07gn6gaour</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:08:23.248</t>
+  </si>
+  <si>
+    <t>77sz8kvuf4lrp79nwq78fa3rvoqsyiby</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:09:24.938</t>
+  </si>
+  <si>
+    <t>5ow5t95g55ktwg4o5ib272mkz4hb46f9</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:10:19.911</t>
+  </si>
+  <si>
+    <t>a9myfe629j000tyjk6y9it69pn548jh8</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:10:43.981</t>
+  </si>
+  <si>
+    <t>u83pzfwmw0y2dv32pn2u08a0c49el785</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:11:05.266</t>
+  </si>
+  <si>
+    <t>o753y1231td9i98nm0xj09kcgyyc4mcx</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:12:22.634</t>
+  </si>
+  <si>
+    <t>x8sl3b0kawx37p1r3380ncvft345fhtr</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:13:23.008</t>
+  </si>
+  <si>
+    <t>vfkp1b0ficw096c7a9qd61o2agd4r3bs</t>
+  </si>
+  <si>
+    <t>2018-11-18T23:13:46.022</t>
+  </si>
+  <si>
+    <t>r03x4a46q2l0kl40y0lrijudc9z2dp7p</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:06:32.448</t>
+  </si>
+  <si>
+    <t>3tn331lbky5lfnz21kvnz296o29c1gei</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:08:59.474</t>
+  </si>
+  <si>
+    <t>z3hf0ttjh6w6eh0579d77fsu212807l2</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:22:45.859</t>
+  </si>
+  <si>
+    <t>h27ryslj2zlc2fsa7yxzjtq3io934eax</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:35:16.460</t>
+  </si>
+  <si>
+    <t>y7w95fdpt119dc75htw67q265rnzg9u2</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:37:35.751</t>
+  </si>
+  <si>
+    <t>zpw2d068dkhd8j70c04bxf22wufe32x3</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:38:27.983</t>
+  </si>
+  <si>
+    <t>06w05idl47014m9k7bht0210dupu0tqp</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:39:58.459</t>
+  </si>
+  <si>
+    <t>98vy7bc017cocl4xc8y301ly873443l9</t>
+  </si>
+  <si>
+    <t>2018-11-19T09:59:15.634</t>
+  </si>
+  <si>
+    <t>wp0fx6f0b0u3u3h38sx1u66kspmoxvrg</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:03:25.772</t>
+  </si>
+  <si>
+    <t>wf0hbuwz2rz7y7pedb43fjr4bwm37ep5</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:06:34.071</t>
+  </si>
+  <si>
+    <t>7103726zmx52hw9ue5nly7o7as19jz84</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:07:24.091</t>
+  </si>
+  <si>
+    <t>82i6qz4d4a1ine80z662g05nu219247b</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:16:00.954</t>
+  </si>
+  <si>
+    <t>i7ly8g68z8c0c883727179s4988o61zg</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:16:29.187</t>
+  </si>
+  <si>
+    <t>5ae9u3b8a0ffq301gsp109h2ko1w2byy</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:17:20.497</t>
+  </si>
+  <si>
+    <t>c1qwkw45g1628410l984834cbylh634g</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:18:31.928</t>
+  </si>
+  <si>
+    <t>wf0972nsj4z31tl2jnxb263cex501ke2</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:20:34.525</t>
+  </si>
+  <si>
+    <t>5u8gdz57yg3p902mx3qeql5q8q9q473c</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:21:21.858</t>
+  </si>
+  <si>
+    <t>cx5q35796sgj1o51gtdw0v5h41u8x9b6</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:22:21.058</t>
+  </si>
+  <si>
+    <t>hs4496v927rf14dln713fhyt8myb480g</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:22:33.623</t>
+  </si>
+  <si>
+    <t>v4j491fard13277ht68dqb1b5b05hlkr</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:22:49.272</t>
+  </si>
+  <si>
+    <t>q85r71m475ld155iux2zx54ug38g1fsp</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:23:30.611</t>
+  </si>
+  <si>
+    <t>kvg92y31mj0x7b05s45t0xw6iiyppy3z</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:25:34.503</t>
+  </si>
+  <si>
+    <t>a43e22b5vfogq37wa7kax069r8oqax00</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:27:36.962</t>
+  </si>
+  <si>
+    <t>qzmbzp90e2z7ct2w904016ptk5b92p40</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:28:06.349</t>
+  </si>
+  <si>
+    <t>un023c9187cm8s28ktz05q6sb733n19i</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:28:35.825</t>
+  </si>
+  <si>
+    <t>kp5sv1uko8lp441p6cki5d37v0fq8k84</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:29:17.042</t>
+  </si>
+  <si>
+    <t>crv0a1nr0301d6uif0i2gwibc2iuhvfm</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:31:25.825</t>
+  </si>
+  <si>
+    <t>7ef2lych652r330wef42wb94trho30ve</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:31:53.812</t>
+  </si>
+  <si>
+    <t>3735qkw8wr7cp1zfiywst012yjtat90i</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:32:22.021</t>
+  </si>
+  <si>
+    <t>94d0j93y78l4vz48tx8k19m1iu712pfa</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:39:53.889</t>
+  </si>
+  <si>
+    <t>5285cuvb23011clvnngh3zlti97yeck3</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:42:22.307</t>
+  </si>
+  <si>
+    <t>jyls88384uwmvt7o36s3f189volr5s4l</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:42:54.065</t>
+  </si>
+  <si>
+    <t>f25fhi3c33j0tg2hs3z06845wu84o0n7</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:43:22.819</t>
+  </si>
+  <si>
+    <t>ak91k7q62ypvcu0zws85dd4eazh9828v</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:43:52.134</t>
+  </si>
+  <si>
+    <t>6m372gtr51j7jpzyaopjbbroj62f235h</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:53:09.315</t>
+  </si>
+  <si>
+    <t>rqlv1erbcz30xj4vtyk8mpfeck7rdjlp</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:53:39.434</t>
+  </si>
+  <si>
+    <t>ctvg02mno75gxvj2524l25s18npxfdsr</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:54:54.595</t>
+  </si>
+  <si>
+    <t>9578yq59gy48gyxn65iiw288hr0qu88p</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:55:19.551</t>
+  </si>
+  <si>
+    <t>599t93wign5ifu7s0x411q9h6p5e88m0</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:56:19.530</t>
+  </si>
+  <si>
+    <t>pldg7ke3ofhbmsp93v3e982d0kyluezb</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:57:19.513</t>
+  </si>
+  <si>
+    <t>k241ytked653p296yrfjelj5v7t1rc15</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:57:31.421</t>
+  </si>
+  <si>
+    <t>sl7f99f8m26k9rfxnbp4zu7ot588h1sf</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:57:43.231</t>
+  </si>
+  <si>
+    <t>o6cxiupx4cnzfl7zj7bwxj5v30yev72h</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:58:23.275</t>
+  </si>
+  <si>
+    <t>ux7wrvcjn3t6024a81qokl7kri518y7f</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:58:35.901</t>
+  </si>
+  <si>
+    <t>u4haef8ns3tdfmyp0xcz4s99t8u15nyy</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:58:49.164</t>
+  </si>
+  <si>
+    <t>41g73k95by6a89k5alhicl2050dc18e3</t>
+  </si>
+  <si>
+    <t>2018-11-19T10:59:23.627</t>
+  </si>
+  <si>
+    <t>778fc96g4xj6df59021214c9sc7q8685</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:00:22.798</t>
+  </si>
+  <si>
+    <t>c1782580vee3ttgl7cc3jbep23f7k7ss</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:00:36.772</t>
+  </si>
+  <si>
+    <t>egvrrlrz6x59ir957sm68mde07i289ja</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:07:22.759</t>
+  </si>
+  <si>
+    <t>2qbqfv3rfj23r6x3sm4ye46p3405dq98</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:08:24.268</t>
+  </si>
+  <si>
+    <t>85gtb93d7szbj6r9mtbfq47t9m64yvhs</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:09:24.620</t>
+  </si>
+  <si>
+    <t>rxd8qd06p7oz238bb7zw3gnt220v7dqk</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:10:20.223</t>
+  </si>
+  <si>
+    <t>9up80h248migbj1q8o2e4b5qv75z1tws</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:12:38.503</t>
+  </si>
+  <si>
+    <t>24a0ya95se7n9qf7f1k40528jq2qcs0j</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:13:22.565</t>
+  </si>
+  <si>
+    <t>c7106287ol5wtqm0879j0zl81fc08y74</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:16:39.024</t>
+  </si>
+  <si>
+    <t>5g4i7c0981209a428c33jimxo8q6g531</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:17:19.021</t>
+  </si>
+  <si>
+    <t>15oel65urzuim20p4w3q7vp040bbdfol</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:17:30.982</t>
+  </si>
+  <si>
+    <t>j8q96k5v7xiai467ogtvp8p4idm5uujc</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:17:42.767</t>
+  </si>
+  <si>
+    <t>947c1prnb8w6za7lsgg52393gcqi7ztl</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:18:21.867</t>
+  </si>
+  <si>
+    <t>q3z0a8q7sf3gcr69b1yv69v12472ffy2</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:20:26.373</t>
+  </si>
+  <si>
+    <t>ks305304319s7gi6d9326ogn09r2vb7a</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:26:51.020</t>
+  </si>
+  <si>
+    <t>adlye1or984uz2p49nx0v7zjbzils290</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:27:21.625</t>
+  </si>
+  <si>
+    <t>0t5kb3284bgbd0zpnur20r9fc7hi30w1</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:29:16.575</t>
+  </si>
+  <si>
+    <t>32u32z6fk1664xe7v77vq3l1l041rc61</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:30:51.807</t>
+  </si>
+  <si>
+    <t>i40wya1i9vo8m8kc8t3pb7fkf0z2ksw3</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:31:22.357</t>
+  </si>
+  <si>
+    <t>8h63i0kv8v8r9q245kqp9z7ry17sv4d2</t>
+  </si>
+  <si>
+    <t>2018-11-19T11:31:37.750</t>
+  </si>
+  <si>
+    <t>w6pix3h20z9wa7f6v86nsfgc9358uewu</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:11:12.166</t>
+  </si>
+  <si>
+    <t>w99xs139303th2q26641gw611s2m7e76</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:13:17.015</t>
+  </si>
+  <si>
+    <t>31z9t666j5v1zdxlbig1aad2v9a9a965</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:15:03.922</t>
+  </si>
+  <si>
+    <t>8n30s2h958z0wxvcl4kn477z91p5p5lk</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:17:16.661</t>
+  </si>
+  <si>
+    <t>u4d29t6i44gz013lp01j99c0ftcbn063</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:19:45.046</t>
+  </si>
+  <si>
+    <t>pwe62z22i6c2w110jz27vv9k6hrfre41</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:21:14.446</t>
+  </si>
+  <si>
+    <t>r1a3sym917jpflkj4m9492m869u3k04j</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:23:13.149</t>
+  </si>
+  <si>
+    <t>okd0omxzda0b6p5i75n65545hq4uhv8q</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:24:23.915</t>
+  </si>
+  <si>
+    <t>b5350npk7g57lh5aeonvd1563v6q3z22</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:24:42.565</t>
+  </si>
+  <si>
+    <t>fqy31y7w1cfwaf0874a98cl012umateg</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:25:23.298</t>
+  </si>
+  <si>
+    <t>mhtw2u26h8vpt8r76wnaf11109nrdj1x</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:27:15.170</t>
+  </si>
+  <si>
+    <t>0qaxrgu4o033fd8ip10a69vszsgr2ruk</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:27:35.295</t>
+  </si>
+  <si>
+    <t>b57v8y2j0jp5bp6319oq8k1b9hulc510</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:30:46.601</t>
+  </si>
+  <si>
+    <t>6xj12ip0f563131kx2w67629304is540</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:33:11.829</t>
+  </si>
+  <si>
+    <t>y9lclv6p93112ahdd9pz3n399dnx8dji</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:34:44.887</t>
+  </si>
+  <si>
+    <t>rlbyp3x0084xknwh70lbk3vopn0cq83y</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:35:20.138</t>
+  </si>
+  <si>
+    <t>mrufk072jb4gr51m3w9ovxp2gxb7vw2i</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:36:23.057</t>
+  </si>
+  <si>
+    <t>lh96wn2bu0e5ifdyr2h9e42mmu5m077l</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:38:13.514</t>
+  </si>
+  <si>
+    <t>g946sgy42jq0a9nre8vtt8n44mf5ub39</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:39:21.574</t>
+  </si>
+  <si>
+    <t>2g7r5jisu3v7343f9j73gu1bu0c39k42</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:39:33.673</t>
+  </si>
+  <si>
+    <t>neq976tggjibw6t6gng8r4104y1yt9h9</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:39:45.770</t>
+  </si>
+  <si>
+    <t>lbwezvsw7vuv2fc7f9qgsh1271xuwj36</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:40:19.746</t>
+  </si>
+  <si>
+    <t>321p9dcplr2fi0gf07chst69t96uc587</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:41:18.712</t>
+  </si>
+  <si>
+    <t>7smq65mo1sop72bhd83fz45i4nh14136</t>
+  </si>
+  <si>
+    <t>2018-11-19T12:41:31.436</t>
+  </si>
+  <si>
+    <t>6a0w8v8vl5z94yqs93l2ye3271umzalg</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:49:49.841</t>
+  </si>
+  <si>
+    <t>ktt1c095yr9qwvaqf57gyqmoiyr85f6k</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:50:22.293</t>
+  </si>
+  <si>
+    <t>24nq3ery00z709qh13da4x45i68xm0eo</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:52:17.406</t>
+  </si>
+  <si>
+    <t>3vwy742cjury53jd55963cimz0mut3m6</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:54:09.626</t>
+  </si>
+  <si>
+    <t>59o4204o3y7sxexfbgeu875605l93xg6</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:56:10.899</t>
+  </si>
+  <si>
+    <t>6vuwy42mp7o9irlf612ktbq4jnxg80yc</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:57:32.816</t>
+  </si>
+  <si>
+    <t>s7f5ow10wf9bt1l07h1m9bvuw2hetrv4</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:58:56.424</t>
+  </si>
+  <si>
+    <t>2tkd0oa09b4b380wz0a8uy6b3vyc9us0</t>
+  </si>
+  <si>
+    <t>2018-11-19T13:59:13.962</t>
+  </si>
+  <si>
+    <t>8k5d22t0211q3pqszpct737160a6lfh5</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:00:19.716</t>
+  </si>
+  <si>
+    <t>5h6p61zl68pt012l7681equluworjm63</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:02:11.940</t>
+  </si>
+  <si>
+    <t>75t1adwapze8961yn9x1p4ze16tzyf0t</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:04:12.735</t>
+  </si>
+  <si>
+    <t>d7b5klbxe46y71dal4lr755u4mybzu5w</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:05:23.022</t>
+  </si>
+  <si>
+    <t>29wope1018kqhn45lse89owq70rva7mi</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:47:07.503</t>
+  </si>
+  <si>
+    <t>ue2rg562ztd45ksezmck098333qbzwer</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:47:19.468</t>
+  </si>
+  <si>
+    <t>j1jp0w5w14lybkixcd2k3484or9f17yo</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:48:23.824</t>
+  </si>
+  <si>
+    <t>p6ti54e122z7tyqsqzdrjfw9o70y161u</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:49:23.168</t>
+  </si>
+  <si>
+    <t>ii7g1f1k73lvi2yff0rifa3781r4yp7s</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:49:35.273</t>
+  </si>
+  <si>
+    <t>54e2e44n53337xs785614zxohbpuud6b</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:50:20.080</t>
+  </si>
+  <si>
+    <t>g63epcgqj3x1keq8i4w335p2dkllpxy3</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:50:32.366</t>
+  </si>
+  <si>
+    <t>4jin79g0ruwf1mo7dt7n2v68pe8cavu6</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:50:44.833</t>
+  </si>
+  <si>
+    <t>5y0p86243v6m48xng4ttcbk6mlvj1fmk</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:50:56.853</t>
+  </si>
+  <si>
+    <t>da8hd3xx75ovd4mzsjz8sf9e637kssrj</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:51:23.398</t>
+  </si>
+  <si>
+    <t>z4nud4939l8dmmluisf7dq2nmgi931bl</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:52:28.606</t>
+  </si>
+  <si>
+    <t>5axzf4cegdkih16rtwzk90enhkz7l0r1</t>
+  </si>
+  <si>
+    <t>2018-11-19T14:52:51.885</t>
+  </si>
+  <si>
+    <t>sned06wvrdbi4x164r5i6qvd45ir672k</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:04:43.770</t>
+  </si>
+  <si>
+    <t>37436f6gq8u2254eo8125a6w795n9l9p</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:05:21.223</t>
+  </si>
+  <si>
+    <t>ay10k3lxxfv8hd5q77md190et655x99o</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:06:22.020</t>
+  </si>
+  <si>
+    <t>62uff02z2v5262j9mnpvptr43b2a0yjl</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:07:21.977</t>
+  </si>
+  <si>
+    <t>lke490ys6fe95o3r488f7m3w146j0hj7</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:08:22.515</t>
+  </si>
+  <si>
+    <t>zi4b7ew6f1qzj385i0ei0793gq884j9x</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:08:44.056</t>
+  </si>
+  <si>
+    <t>4ncn0r8rk8c98c23e1dqrhjtkdq14enc</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:09:08.819</t>
+  </si>
+  <si>
+    <t>99ooof4y890i1i7k2if9ze8ftr5662re</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:23:07.897</t>
+  </si>
+  <si>
+    <t>mx773bf76z9201e35kok418ntkc6msj7</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:24:25.324</t>
+  </si>
+  <si>
+    <t>uelhqzz4lbo22p6anfow661idb2nc761</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:26:39.668</t>
+  </si>
+  <si>
+    <t>exo93hwm69cf96ori48s2oih7e2o23j7</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:27:33.098</t>
+  </si>
+  <si>
+    <t>x9fjnre7ydyz81csrd7cbvwnu9ob8kq1</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:28:21.951</t>
+  </si>
+  <si>
+    <t>4wd6o53gz84774l8ix219c0vzbi5w73d</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:29:24.423</t>
+  </si>
+  <si>
+    <t>50usew49osr7oy4wo6rwm4z3i8mn02a6</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:30:22.188</t>
+  </si>
+  <si>
+    <t>akmb25z65ups22p607qovb4ut09jjd7a</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:30:47.041</t>
+  </si>
+  <si>
+    <t>0x0u4g257vgro64umel3bb3mtsgiv8pd</t>
+  </si>
+  <si>
+    <t>2018-11-19T15:31:09.736</t>
   </si>
 </sst>
 </file>
@@ -5624,6 +7034,1886 @@
         <v>747</v>
       </c>
     </row>
+    <row r="376">
+      <c r="A376" t="s">
+        <v>748</v>
+      </c>
+      <c r="B376" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s">
+        <v>750</v>
+      </c>
+      <c r="B377" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s">
+        <v>752</v>
+      </c>
+      <c r="B378" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s">
+        <v>754</v>
+      </c>
+      <c r="B379" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s">
+        <v>756</v>
+      </c>
+      <c r="B380" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s">
+        <v>758</v>
+      </c>
+      <c r="B381" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s">
+        <v>760</v>
+      </c>
+      <c r="B382" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s">
+        <v>762</v>
+      </c>
+      <c r="B383" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s">
+        <v>764</v>
+      </c>
+      <c r="B384" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s">
+        <v>766</v>
+      </c>
+      <c r="B385" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s">
+        <v>768</v>
+      </c>
+      <c r="B386" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s">
+        <v>770</v>
+      </c>
+      <c r="B387" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s">
+        <v>772</v>
+      </c>
+      <c r="B388" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="s">
+        <v>774</v>
+      </c>
+      <c r="B389" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="s">
+        <v>776</v>
+      </c>
+      <c r="B390" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="s">
+        <v>778</v>
+      </c>
+      <c r="B391" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="s">
+        <v>780</v>
+      </c>
+      <c r="B392" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="s">
+        <v>782</v>
+      </c>
+      <c r="B393" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="s">
+        <v>784</v>
+      </c>
+      <c r="B394" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="s">
+        <v>786</v>
+      </c>
+      <c r="B395" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="s">
+        <v>788</v>
+      </c>
+      <c r="B396" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="s">
+        <v>790</v>
+      </c>
+      <c r="B397" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="s">
+        <v>792</v>
+      </c>
+      <c r="B398" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="s">
+        <v>794</v>
+      </c>
+      <c r="B399" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="s">
+        <v>796</v>
+      </c>
+      <c r="B400" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="s">
+        <v>798</v>
+      </c>
+      <c r="B401" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="s">
+        <v>800</v>
+      </c>
+      <c r="B402" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="s">
+        <v>802</v>
+      </c>
+      <c r="B403" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="s">
+        <v>804</v>
+      </c>
+      <c r="B404" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="s">
+        <v>806</v>
+      </c>
+      <c r="B405" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="s">
+        <v>808</v>
+      </c>
+      <c r="B406" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="s">
+        <v>810</v>
+      </c>
+      <c r="B407" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="s">
+        <v>812</v>
+      </c>
+      <c r="B408" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="s">
+        <v>814</v>
+      </c>
+      <c r="B409" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="s">
+        <v>816</v>
+      </c>
+      <c r="B410" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="s">
+        <v>818</v>
+      </c>
+      <c r="B411" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="s">
+        <v>820</v>
+      </c>
+      <c r="B412" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="s">
+        <v>822</v>
+      </c>
+      <c r="B413" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="s">
+        <v>824</v>
+      </c>
+      <c r="B414" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="s">
+        <v>826</v>
+      </c>
+      <c r="B415" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="s">
+        <v>828</v>
+      </c>
+      <c r="B416" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="s">
+        <v>830</v>
+      </c>
+      <c r="B417" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="s">
+        <v>832</v>
+      </c>
+      <c r="B418" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="s">
+        <v>834</v>
+      </c>
+      <c r="B419" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="s">
+        <v>836</v>
+      </c>
+      <c r="B420" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="s">
+        <v>838</v>
+      </c>
+      <c r="B421" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="s">
+        <v>840</v>
+      </c>
+      <c r="B422" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="s">
+        <v>842</v>
+      </c>
+      <c r="B423" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="s">
+        <v>844</v>
+      </c>
+      <c r="B424" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="s">
+        <v>846</v>
+      </c>
+      <c r="B425" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="s">
+        <v>848</v>
+      </c>
+      <c r="B426" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="s">
+        <v>850</v>
+      </c>
+      <c r="B427" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="s">
+        <v>852</v>
+      </c>
+      <c r="B428" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="s">
+        <v>854</v>
+      </c>
+      <c r="B429" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="s">
+        <v>856</v>
+      </c>
+      <c r="B430" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="s">
+        <v>858</v>
+      </c>
+      <c r="B431" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="s">
+        <v>860</v>
+      </c>
+      <c r="B432" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="s">
+        <v>862</v>
+      </c>
+      <c r="B433" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="s">
+        <v>864</v>
+      </c>
+      <c r="B434" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="s">
+        <v>866</v>
+      </c>
+      <c r="B435" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="s">
+        <v>868</v>
+      </c>
+      <c r="B436" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="s">
+        <v>870</v>
+      </c>
+      <c r="B437" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="s">
+        <v>872</v>
+      </c>
+      <c r="B438" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="s">
+        <v>874</v>
+      </c>
+      <c r="B439" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="s">
+        <v>876</v>
+      </c>
+      <c r="B440" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="s">
+        <v>878</v>
+      </c>
+      <c r="B441" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="s">
+        <v>880</v>
+      </c>
+      <c r="B442" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="s">
+        <v>882</v>
+      </c>
+      <c r="B443" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="s">
+        <v>884</v>
+      </c>
+      <c r="B444" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="s">
+        <v>886</v>
+      </c>
+      <c r="B445" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="s">
+        <v>888</v>
+      </c>
+      <c r="B446" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="s">
+        <v>890</v>
+      </c>
+      <c r="B447" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="s">
+        <v>892</v>
+      </c>
+      <c r="B448" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="s">
+        <v>894</v>
+      </c>
+      <c r="B449" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="s">
+        <v>896</v>
+      </c>
+      <c r="B450" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="s">
+        <v>898</v>
+      </c>
+      <c r="B451" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="s">
+        <v>900</v>
+      </c>
+      <c r="B452" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="s">
+        <v>902</v>
+      </c>
+      <c r="B453" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="s">
+        <v>904</v>
+      </c>
+      <c r="B454" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="s">
+        <v>906</v>
+      </c>
+      <c r="B455" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="s">
+        <v>908</v>
+      </c>
+      <c r="B456" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="s">
+        <v>910</v>
+      </c>
+      <c r="B457" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="s">
+        <v>912</v>
+      </c>
+      <c r="B458" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="s">
+        <v>914</v>
+      </c>
+      <c r="B459" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="s">
+        <v>916</v>
+      </c>
+      <c r="B460" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="s">
+        <v>918</v>
+      </c>
+      <c r="B461" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="s">
+        <v>920</v>
+      </c>
+      <c r="B462" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="s">
+        <v>922</v>
+      </c>
+      <c r="B463" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="s">
+        <v>924</v>
+      </c>
+      <c r="B464" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="s">
+        <v>926</v>
+      </c>
+      <c r="B465" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="s">
+        <v>928</v>
+      </c>
+      <c r="B466" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="s">
+        <v>930</v>
+      </c>
+      <c r="B467" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="s">
+        <v>932</v>
+      </c>
+      <c r="B468" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="s">
+        <v>934</v>
+      </c>
+      <c r="B469" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="s">
+        <v>936</v>
+      </c>
+      <c r="B470" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="s">
+        <v>938</v>
+      </c>
+      <c r="B471" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="s">
+        <v>940</v>
+      </c>
+      <c r="B472" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="s">
+        <v>942</v>
+      </c>
+      <c r="B473" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="s">
+        <v>944</v>
+      </c>
+      <c r="B474" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="s">
+        <v>946</v>
+      </c>
+      <c r="B475" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="s">
+        <v>948</v>
+      </c>
+      <c r="B476" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="s">
+        <v>950</v>
+      </c>
+      <c r="B477" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="s">
+        <v>952</v>
+      </c>
+      <c r="B478" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="s">
+        <v>954</v>
+      </c>
+      <c r="B479" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="s">
+        <v>956</v>
+      </c>
+      <c r="B480" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="s">
+        <v>958</v>
+      </c>
+      <c r="B481" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="s">
+        <v>960</v>
+      </c>
+      <c r="B482" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="s">
+        <v>962</v>
+      </c>
+      <c r="B483" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="s">
+        <v>964</v>
+      </c>
+      <c r="B484" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="s">
+        <v>966</v>
+      </c>
+      <c r="B485" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="s">
+        <v>968</v>
+      </c>
+      <c r="B486" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="s">
+        <v>970</v>
+      </c>
+      <c r="B487" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="s">
+        <v>972</v>
+      </c>
+      <c r="B488" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="s">
+        <v>974</v>
+      </c>
+      <c r="B489" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="s">
+        <v>976</v>
+      </c>
+      <c r="B490" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="s">
+        <v>978</v>
+      </c>
+      <c r="B491" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="s">
+        <v>980</v>
+      </c>
+      <c r="B492" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="s">
+        <v>982</v>
+      </c>
+      <c r="B493" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="s">
+        <v>984</v>
+      </c>
+      <c r="B494" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="s">
+        <v>986</v>
+      </c>
+      <c r="B495" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="s">
+        <v>988</v>
+      </c>
+      <c r="B496" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="s">
+        <v>990</v>
+      </c>
+      <c r="B497" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="s">
+        <v>992</v>
+      </c>
+      <c r="B498" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="s">
+        <v>994</v>
+      </c>
+      <c r="B499" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="s">
+        <v>996</v>
+      </c>
+      <c r="B500" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="s">
+        <v>998</v>
+      </c>
+      <c r="B501" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B502" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B507" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B508" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B509" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B510" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B511" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B512" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B513" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B516" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B517" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B518" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B519" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B520" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B521" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B522" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B523" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B524" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B525" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B526" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B527" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B528" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B529" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B531" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B533" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B534" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B535" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B536" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B537" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B538" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B540" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B541" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B542" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B543" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B544" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B545" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B546" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B547" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B549" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B552" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B554" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B556" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B557" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B559" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B560" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B561" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B562" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B563" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B564" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B565" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B566" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B567" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B568" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B569" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B570" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B571" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B572" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B573" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B574" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B575" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B576" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B577" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B579" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B580" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B582" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B585" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B586" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B587" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B588" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B589" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B590" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B591" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B592" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B593" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B594" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B595" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B596" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B597" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B598" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B599" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B600" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B601" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B602" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B603" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B604" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B605" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B606" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B607" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B608" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B609" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B610" t="s">
+        <v>1217</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Changing pom to run with plugin maven-compiler
</commit_message>
<xml_diff>
--- a/src/main/java/resources/generateduuid.xlsx
+++ b/src/main/java/resources/generateduuid.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5575" uniqueCount="4067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5579" uniqueCount="4071">
   <si>
     <t>Vehicle uuid</t>
   </si>
@@ -12227,6 +12227,18 @@
   </si>
   <si>
     <t>2018-12-02T09:17:28.462</t>
+  </si>
+  <si>
+    <t>xdiyh9wl264d20l7624u6dt0o6bx3vil0a5</t>
+  </si>
+  <si>
+    <t>2018-12-02T20:22:09.566</t>
+  </si>
+  <si>
+    <t>r8re11gesbf1gxilawcpzjjoei6y2jk3r0a</t>
+  </si>
+  <si>
+    <t>2018-12-02T20:22:39.330</t>
   </si>
 </sst>
 </file>
@@ -25070,6 +25082,22 @@
         <v>4066</v>
       </c>
     </row>
+    <row r="1562">
+      <c r="A1562" t="s">
+        <v>4067</v>
+      </c>
+      <c r="B1562" t="s">
+        <v>4068</v>
+      </c>
+    </row>
+    <row r="1563">
+      <c r="A1563" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B1563" t="s">
+        <v>4070</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added RestApi part with 5-6 endpoints
</commit_message>
<xml_diff>
--- a/src/main/java/resources/generateduuid.xlsx
+++ b/src/main/java/resources/generateduuid.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12374" uniqueCount="7911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12930" uniqueCount="8189">
   <si>
     <t>Vehicle uuid</t>
   </si>
@@ -23759,6 +23759,840 @@
   </si>
   <si>
     <t>2018-12-15T13:23:18.190</t>
+  </si>
+  <si>
+    <t>2018-12-22T13:24:05</t>
+  </si>
+  <si>
+    <t>2018-12-15T16:20:46.533</t>
+  </si>
+  <si>
+    <t>q76bd2li7b552evgf0pv0c57734zl2c600z</t>
+  </si>
+  <si>
+    <t>2018-12-15T16:20:50.401</t>
+  </si>
+  <si>
+    <t>eao15w0t6j1z2f6167is8mzmro47080g9z6</t>
+  </si>
+  <si>
+    <t>2018-12-15T16:21:05.105</t>
+  </si>
+  <si>
+    <t>0y3suup4ia30x0qsrk57ztl06ubsq064a0m</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:02:25.318</t>
+  </si>
+  <si>
+    <t>0s0m4ooiqmus7r671d1nomy0ng34p9rpf6w</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:02:27.070</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:02:33</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:03:06.013</t>
+  </si>
+  <si>
+    <t>WBAJE7C59KWW16413</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:02:32</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:03:08.115</t>
+  </si>
+  <si>
+    <t>65zxz25azal3d32f0mm8y959cup134n87hf</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:03:12.417</t>
+  </si>
+  <si>
+    <t>2018-12-24T09:03:07</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:09.080</t>
+  </si>
+  <si>
+    <t>2018-12-24T09:03:12</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:09.769</t>
+  </si>
+  <si>
+    <t>5UXKR2C59J0Z15155</t>
+  </si>
+  <si>
+    <t>2018-12-24T09:04:06</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:10.492</t>
+  </si>
+  <si>
+    <t>zy73to1wnyfz1632c1i9h4f8wc719a42vsc</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:14.583</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:21</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:38.409</t>
+  </si>
+  <si>
+    <t>t68d1o7eh7xdyokgk0s66ddx7s01d39u3zy</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:04:42.170</t>
+  </si>
+  <si>
+    <t>2018-12-24T09:05:07</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:18:03.143</t>
+  </si>
+  <si>
+    <t>xxk35emwm8v1pf2hj0w60q8otv86fzvd8n4</t>
+  </si>
+  <si>
+    <t>2018-12-17T09:18:19.269</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111110</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:10:08</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:52.027</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111111</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:10:07</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:52.997</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111112</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:53.740</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111113</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:54.429</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111114</t>
+  </si>
+  <si>
+    <t>WBXHT3C30J5L34022</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:55.059</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111115</t>
+  </si>
+  <si>
+    <t>WBA4J3C54KBL07084</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:55.698</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111116</t>
+  </si>
+  <si>
+    <t>5UXKR0C50J0X88087</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:11:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:56.333</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111117</t>
+  </si>
+  <si>
+    <t>5UXTS3C53J0Z02433</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:11:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:56.948</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111118</t>
+  </si>
+  <si>
+    <t>5UXTR7C54KLF33720</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:11:07</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:57.623</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111119</t>
+  </si>
+  <si>
+    <t>5UXTR7C53KLF33725</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:58.231</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111120</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:12:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:58.860</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111121</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:12:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:58:59.471</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111122</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:00.147</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111123</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:00.773</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111124</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:13:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:01.391</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111125</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:13:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:02.029</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111126</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:02.653</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111127</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:14:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:03.280</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111128</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:03.943</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111129</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:15:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:04.558</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111130</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:05.179</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111131</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:16:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:05.819</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111132</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:17:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:06.435</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111133</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:18:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:07.044</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111134</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:19:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:07.696</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111135</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:20:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:08.303</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111136</t>
+  </si>
+  <si>
+    <t>2018-12-24T21:00:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:08.916</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111137</t>
+  </si>
+  <si>
+    <t>2018-12-17T21:00:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:09.538</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111138</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:10.179</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111139</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:10.803</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111110</t>
+  </si>
+  <si>
+    <t>WBA8A9C52JAH12047</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:11.412</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111111</t>
+  </si>
+  <si>
+    <t>WBA8B9G59JNU99692</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:12.032</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111112</t>
+  </si>
+  <si>
+    <t>2018-12-17T20:10:09</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:12.715</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111113</t>
+  </si>
+  <si>
+    <t>WBA8E1C5XJA756445</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:13.325</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111114</t>
+  </si>
+  <si>
+    <t>5UXKR2C55J0Z22121</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:13.933</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111115</t>
+  </si>
+  <si>
+    <t>5UXTS3C57K0Z04834</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:14.544</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111116</t>
+  </si>
+  <si>
+    <t>WBAJA7C58KWW06127</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:15.193</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111117</t>
+  </si>
+  <si>
+    <t>WBAJA7C56KWW11990</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:15.815</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111118</t>
+  </si>
+  <si>
+    <t>WBA7F2C59KB240233</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:16.437</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111119</t>
+  </si>
+  <si>
+    <t>WBA8A3C58JA505978</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:17.045</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111120</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:17.654</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111121</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:18.315</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111122</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:18.926</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111123</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:19.534</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111124</t>
+  </si>
+  <si>
+    <t>2018-12-24T20:10:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:20.147</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111125</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:20.757</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111126</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:21.412</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111127</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:22.031</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111128</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:22.645</t>
+  </si>
+  <si>
+    <t>21111111111111111111111111111111129</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:23.258</t>
+  </si>
+  <si>
+    <t>fy3axfm585y5y2t7xke02oqw2sswf1qrmy7</t>
+  </si>
+  <si>
+    <t>2018-12-18T15:59:26.688</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:00:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:00:08.910</t>
+  </si>
+  <si>
+    <t>230wo6aqczg335bbgz398as41n5fi3j8c9f</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:00:12.323</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:01:07</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:09.779</t>
+  </si>
+  <si>
+    <t>4521md68nr3qvhdl1525m2wt62jc79p207f</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:13.273</t>
+  </si>
+  <si>
+    <t>a5db68bb0a0e0adf052ed355793a2935zfa</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:18.195</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:19</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:26.064</t>
+  </si>
+  <si>
+    <t>kloi10ms8vx84nw9w659sfkla9bd0b2fo1x</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:29.497</t>
+  </si>
+  <si>
+    <t>d4348fe40a0e0a17623e2bddc20b7fc2gx0</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:35.155</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:36</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:43.046</t>
+  </si>
+  <si>
+    <t>y720pb515nn12z5cfj81ac84jm4qfka6i5e</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:01:46.382</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:02:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:02:08.707</t>
+  </si>
+  <si>
+    <t>1k4a60101v801hl5z4g7r97f1k5007rw2dr</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:02:12.060</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:03:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:03:08.667</t>
+  </si>
+  <si>
+    <t>7hrtja6w3fog50dt7my1f0590q5gikba9q7</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:03:12.034</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:04:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:04:08.879</t>
+  </si>
+  <si>
+    <t>1x2u96c84w60y844hri93sp0crg3fnbwqem</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:04:12.267</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:05:05</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:08.752</t>
+  </si>
+  <si>
+    <t>qlwnf65lrbxr7qx43390o7aru109s7m3632</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:12.259</t>
+  </si>
+  <si>
+    <t>5UXKU2C55K0Z64000</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:21</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:25.372</t>
+  </si>
+  <si>
+    <t>s9b7x53lb53qrok5ddn0vp0756lhy783jnu</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:28.915</t>
+  </si>
+  <si>
+    <t>WAU24GF56JN009862</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:35</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:39.934</t>
+  </si>
+  <si>
+    <t>dq595d09mbz29135kzn6k689rl0e4dvfsb8</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:44.011</t>
+  </si>
+  <si>
+    <t>5UXTR9C51KLE12400</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:05:52</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:01.497</t>
+  </si>
+  <si>
+    <t>pratbi3fzy2jy4wqrey0uh6m4kk0hw8586u</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:05.771</t>
+  </si>
+  <si>
+    <t>WBS3S7C59KAC09544</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:19</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:26.247</t>
+  </si>
+  <si>
+    <t>7y1f2y3178nnd66l3ce1124970098e4wv0u</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:29.839</t>
+  </si>
+  <si>
+    <t>WBXHT3C33J5L30966</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:39</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:45.983</t>
+  </si>
+  <si>
+    <t>8hcqyup12n8d6yxv70y47hc75zg1xr19829</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:06:49.812</t>
+  </si>
+  <si>
+    <t>WAUPNAF53JA084008</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:07:17</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:07:24.738</t>
+  </si>
+  <si>
+    <t>ultrq1942i4yw14xed5yg91mervsghiucne</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:07:28.364</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:07:36</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:07:43.047</t>
+  </si>
+  <si>
+    <t>3tfvutws1923n84d46i031x8odfkm12p39g</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:07:46.816</t>
+  </si>
+  <si>
+    <t>WA1VAAF72JD027511</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:08:14</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:08:21.483</t>
+  </si>
+  <si>
+    <t>o389xhlb21qh89j556s5vt06bxo6w9pumy6</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:08:25.355</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:08:54</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:08:59.864</t>
+  </si>
+  <si>
+    <t>49z2q02wqmedqfbxf2b2khz5255q5yih971</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:09:03.564</t>
+  </si>
+  <si>
+    <t>WBXHT3C38J5F92260</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:09:31</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:09:36.529</t>
+  </si>
+  <si>
+    <t>2pgs4ftpws74e3wz5p0i1m3065132alqj7o</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:09:40.157</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:11:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:11:10.604</t>
+  </si>
+  <si>
+    <t>ug349636054hi31zg21iadrh63oeqtpgox7</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:11:14.323</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:12:06</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:12:10.271</t>
+  </si>
+  <si>
+    <t>u8n69z8lks1y4ns011i2q73wp9k9l7ti68t</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:12:14.312</t>
+  </si>
+  <si>
+    <t>3bd9dc580a0a00de6a568762d66fa01av7m</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:12:35.003</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:13:05</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:13:09.755</t>
+  </si>
+  <si>
+    <t>ntan8br55kdx8nsjwyhu955nh6h73lie1bn</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:13:13.189</t>
+  </si>
+  <si>
+    <t>04c16ffd0a0e0adf4d75c02155d62aedh50</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:13:17.774</t>
+  </si>
+  <si>
+    <t>2018-12-25T16:14:05</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:15:19.757</t>
+  </si>
+  <si>
+    <t>5tvrufjv86rdf7b695rf14a4okyh7354v7w</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:15:23.667</t>
+  </si>
+  <si>
+    <t>WBXHT3C38J5K24335</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:16:10</t>
+  </si>
+  <si>
+    <t>2018-12-18T16:16:11.661</t>
   </si>
 </sst>
 </file>
@@ -51204,6 +52038,286 @@
         <v>7910</v>
       </c>
     </row>
+    <row r="2573">
+      <c r="A2573" t="s">
+        <v>7913</v>
+      </c>
+      <c r="B2573" t="s">
+        <v>7914</v>
+      </c>
+    </row>
+    <row r="2574">
+      <c r="A2574" t="s">
+        <v>7915</v>
+      </c>
+      <c r="B2574" t="s">
+        <v>7916</v>
+      </c>
+    </row>
+    <row r="2575">
+      <c r="A2575" t="s">
+        <v>7917</v>
+      </c>
+      <c r="B2575" t="s">
+        <v>7918</v>
+      </c>
+    </row>
+    <row r="2576">
+      <c r="A2576" t="s">
+        <v>7919</v>
+      </c>
+      <c r="B2576" t="s">
+        <v>7920</v>
+      </c>
+    </row>
+    <row r="2577">
+      <c r="A2577" t="s">
+        <v>7926</v>
+      </c>
+      <c r="B2577" t="s">
+        <v>7927</v>
+      </c>
+    </row>
+    <row r="2578">
+      <c r="A2578" t="s">
+        <v>7935</v>
+      </c>
+      <c r="B2578" t="s">
+        <v>7936</v>
+      </c>
+    </row>
+    <row r="2579">
+      <c r="A2579" t="s">
+        <v>7939</v>
+      </c>
+      <c r="B2579" t="s">
+        <v>7940</v>
+      </c>
+    </row>
+    <row r="2580">
+      <c r="A2580" t="s">
+        <v>7943</v>
+      </c>
+      <c r="B2580" t="s">
+        <v>7944</v>
+      </c>
+    </row>
+    <row r="2581">
+      <c r="A2581" t="s">
+        <v>8080</v>
+      </c>
+      <c r="B2581" t="s">
+        <v>8081</v>
+      </c>
+    </row>
+    <row r="2582">
+      <c r="A2582" t="s">
+        <v>8084</v>
+      </c>
+      <c r="B2582" t="s">
+        <v>8085</v>
+      </c>
+    </row>
+    <row r="2583">
+      <c r="A2583" t="s">
+        <v>8088</v>
+      </c>
+      <c r="B2583" t="s">
+        <v>8089</v>
+      </c>
+    </row>
+    <row r="2584">
+      <c r="A2584" t="s">
+        <v>8090</v>
+      </c>
+      <c r="B2584" t="s">
+        <v>8091</v>
+      </c>
+    </row>
+    <row r="2585">
+      <c r="A2585" t="s">
+        <v>8094</v>
+      </c>
+      <c r="B2585" t="s">
+        <v>8095</v>
+      </c>
+    </row>
+    <row r="2586">
+      <c r="A2586" t="s">
+        <v>8096</v>
+      </c>
+      <c r="B2586" t="s">
+        <v>8097</v>
+      </c>
+    </row>
+    <row r="2587">
+      <c r="A2587" t="s">
+        <v>8100</v>
+      </c>
+      <c r="B2587" t="s">
+        <v>8101</v>
+      </c>
+    </row>
+    <row r="2588">
+      <c r="A2588" t="s">
+        <v>8104</v>
+      </c>
+      <c r="B2588" t="s">
+        <v>8105</v>
+      </c>
+    </row>
+    <row r="2589">
+      <c r="A2589" t="s">
+        <v>8108</v>
+      </c>
+      <c r="B2589" t="s">
+        <v>8109</v>
+      </c>
+    </row>
+    <row r="2590">
+      <c r="A2590" t="s">
+        <v>8112</v>
+      </c>
+      <c r="B2590" t="s">
+        <v>8113</v>
+      </c>
+    </row>
+    <row r="2591">
+      <c r="A2591" t="s">
+        <v>8116</v>
+      </c>
+      <c r="B2591" t="s">
+        <v>8117</v>
+      </c>
+    </row>
+    <row r="2592">
+      <c r="A2592" t="s">
+        <v>8121</v>
+      </c>
+      <c r="B2592" t="s">
+        <v>8122</v>
+      </c>
+    </row>
+    <row r="2593">
+      <c r="A2593" t="s">
+        <v>8126</v>
+      </c>
+      <c r="B2593" t="s">
+        <v>8127</v>
+      </c>
+    </row>
+    <row r="2594">
+      <c r="A2594" t="s">
+        <v>8131</v>
+      </c>
+      <c r="B2594" t="s">
+        <v>8132</v>
+      </c>
+    </row>
+    <row r="2595">
+      <c r="A2595" t="s">
+        <v>8136</v>
+      </c>
+      <c r="B2595" t="s">
+        <v>8137</v>
+      </c>
+    </row>
+    <row r="2596">
+      <c r="A2596" t="s">
+        <v>8141</v>
+      </c>
+      <c r="B2596" t="s">
+        <v>8142</v>
+      </c>
+    </row>
+    <row r="2597">
+      <c r="A2597" t="s">
+        <v>8146</v>
+      </c>
+      <c r="B2597" t="s">
+        <v>8147</v>
+      </c>
+    </row>
+    <row r="2598">
+      <c r="A2598" t="s">
+        <v>8150</v>
+      </c>
+      <c r="B2598" t="s">
+        <v>8151</v>
+      </c>
+    </row>
+    <row r="2599">
+      <c r="A2599" t="s">
+        <v>8155</v>
+      </c>
+      <c r="B2599" t="s">
+        <v>8156</v>
+      </c>
+    </row>
+    <row r="2600">
+      <c r="A2600" t="s">
+        <v>8159</v>
+      </c>
+      <c r="B2600" t="s">
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="2601">
+      <c r="A2601" t="s">
+        <v>8164</v>
+      </c>
+      <c r="B2601" t="s">
+        <v>8165</v>
+      </c>
+    </row>
+    <row r="2602">
+      <c r="A2602" t="s">
+        <v>8168</v>
+      </c>
+      <c r="B2602" t="s">
+        <v>8169</v>
+      </c>
+    </row>
+    <row r="2603">
+      <c r="A2603" t="s">
+        <v>8172</v>
+      </c>
+      <c r="B2603" t="s">
+        <v>8173</v>
+      </c>
+    </row>
+    <row r="2604">
+      <c r="A2604" t="s">
+        <v>8174</v>
+      </c>
+      <c r="B2604" t="s">
+        <v>8175</v>
+      </c>
+    </row>
+    <row r="2605">
+      <c r="A2605" t="s">
+        <v>8178</v>
+      </c>
+      <c r="B2605" t="s">
+        <v>8179</v>
+      </c>
+    </row>
+    <row r="2606">
+      <c r="A2606" t="s">
+        <v>8180</v>
+      </c>
+      <c r="B2606" t="s">
+        <v>8181</v>
+      </c>
+    </row>
+    <row r="2607">
+      <c r="A2607" t="s">
+        <v>8184</v>
+      </c>
+      <c r="B2607" t="s">
+        <v>8185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -84645,6 +85759,2112 @@
         <v>7906</v>
       </c>
     </row>
+    <row r="1209">
+      <c r="A1209" t="s">
+        <v>7909</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1209" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1209" t="s">
+        <v>7911</v>
+      </c>
+      <c r="F1209" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1209" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1209" t="s">
+        <v>7912</v>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="s">
+        <v>7919</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>5953</v>
+      </c>
+      <c r="D1210" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1210" t="s">
+        <v>7921</v>
+      </c>
+      <c r="F1210" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1210" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1210" t="s">
+        <v>7922</v>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="s">
+        <v>7917</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1211" t="s">
+        <v>7923</v>
+      </c>
+      <c r="D1211" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1211" t="s">
+        <v>7924</v>
+      </c>
+      <c r="F1211" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G1211" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1211" t="s">
+        <v>7925</v>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="s">
+        <v>7919</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1212" t="s">
+        <v>5953</v>
+      </c>
+      <c r="D1212" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1212" t="s">
+        <v>7928</v>
+      </c>
+      <c r="F1212" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1212" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1212" t="s">
+        <v>7929</v>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="s">
+        <v>7917</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>2149</v>
+      </c>
+      <c r="C1213" t="s">
+        <v>7923</v>
+      </c>
+      <c r="D1213" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1213" t="s">
+        <v>7930</v>
+      </c>
+      <c r="F1213" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G1213" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1213" t="s">
+        <v>7931</v>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="s">
+        <v>7926</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1214" t="s">
+        <v>7932</v>
+      </c>
+      <c r="D1214" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1214" t="s">
+        <v>7933</v>
+      </c>
+      <c r="F1214" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1214" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1214" t="s">
+        <v>7934</v>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="s">
+        <v>7935</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1215" t="s">
+        <v>7923</v>
+      </c>
+      <c r="D1215" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1215" t="s">
+        <v>7937</v>
+      </c>
+      <c r="F1215" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1215" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1215" t="s">
+        <v>7938</v>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="s">
+        <v>7939</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1216" t="s">
+        <v>7482</v>
+      </c>
+      <c r="D1216" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1216" t="s">
+        <v>7941</v>
+      </c>
+      <c r="F1216" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1216" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1216" t="s">
+        <v>7942</v>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="s">
+        <v>7945</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1217" t="s">
+        <v>2826</v>
+      </c>
+      <c r="D1217" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1217" t="s">
+        <v>7946</v>
+      </c>
+      <c r="F1217" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1217" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1217" t="s">
+        <v>7947</v>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="s">
+        <v>7948</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1218" t="s">
+        <v>3651</v>
+      </c>
+      <c r="D1218" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1218" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1218" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1218" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1218" t="s">
+        <v>7950</v>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="s">
+        <v>7951</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1219" t="s">
+        <v>5203</v>
+      </c>
+      <c r="D1219" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1219" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1219" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1219" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1219" t="s">
+        <v>7952</v>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="s">
+        <v>7953</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1220" t="s">
+        <v>3970</v>
+      </c>
+      <c r="D1220" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1220" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1220" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1220" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1220" t="s">
+        <v>7954</v>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="s">
+        <v>7955</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>7956</v>
+      </c>
+      <c r="D1221" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1221" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1221" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1221" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1221" t="s">
+        <v>7957</v>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="s">
+        <v>7958</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>7959</v>
+      </c>
+      <c r="D1222" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1222" t="s">
+        <v>7946</v>
+      </c>
+      <c r="F1222" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1222" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1222" t="s">
+        <v>7960</v>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="s">
+        <v>7961</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>7962</v>
+      </c>
+      <c r="D1223" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1223" t="s">
+        <v>7963</v>
+      </c>
+      <c r="F1223" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1223" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1223" t="s">
+        <v>7964</v>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="s">
+        <v>7965</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>7966</v>
+      </c>
+      <c r="D1224" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1224" t="s">
+        <v>7967</v>
+      </c>
+      <c r="F1224" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1224" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1224" t="s">
+        <v>7968</v>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="s">
+        <v>7969</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>7970</v>
+      </c>
+      <c r="D1225" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1225" t="s">
+        <v>7971</v>
+      </c>
+      <c r="F1225" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1225" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1225" t="s">
+        <v>7972</v>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="s">
+        <v>7973</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>7974</v>
+      </c>
+      <c r="D1226" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1226" t="s">
+        <v>7971</v>
+      </c>
+      <c r="F1226" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1226" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1226" t="s">
+        <v>7975</v>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="s">
+        <v>7976</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>2826</v>
+      </c>
+      <c r="D1227" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1227" t="s">
+        <v>7977</v>
+      </c>
+      <c r="F1227" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1227" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1227" t="s">
+        <v>7978</v>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="s">
+        <v>7979</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>3651</v>
+      </c>
+      <c r="D1228" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1228" t="s">
+        <v>7980</v>
+      </c>
+      <c r="F1228" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1228" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1228" t="s">
+        <v>7981</v>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="s">
+        <v>7982</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>5203</v>
+      </c>
+      <c r="D1229" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1229" t="s">
+        <v>7980</v>
+      </c>
+      <c r="F1229" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1229" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1229" t="s">
+        <v>7983</v>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="s">
+        <v>7984</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>3970</v>
+      </c>
+      <c r="D1230" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1230" t="s">
+        <v>7980</v>
+      </c>
+      <c r="F1230" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1230" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1230" t="s">
+        <v>7985</v>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="s">
+        <v>7986</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>7956</v>
+      </c>
+      <c r="D1231" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1231" t="s">
+        <v>7987</v>
+      </c>
+      <c r="F1231" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1231" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1231" t="s">
+        <v>7988</v>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="s">
+        <v>7989</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>7959</v>
+      </c>
+      <c r="D1232" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1232" t="s">
+        <v>7990</v>
+      </c>
+      <c r="F1232" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1232" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1232" t="s">
+        <v>7991</v>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="s">
+        <v>7992</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>7962</v>
+      </c>
+      <c r="D1233" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1233" t="s">
+        <v>7987</v>
+      </c>
+      <c r="F1233" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1233" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1233" t="s">
+        <v>7993</v>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="s">
+        <v>7994</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>7966</v>
+      </c>
+      <c r="D1234" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1234" t="s">
+        <v>7995</v>
+      </c>
+      <c r="F1234" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1234" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1234" t="s">
+        <v>7996</v>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="s">
+        <v>7997</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1235" t="s">
+        <v>7970</v>
+      </c>
+      <c r="D1235" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1235" t="s">
+        <v>7995</v>
+      </c>
+      <c r="F1235" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1235" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1235" t="s">
+        <v>7998</v>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="s">
+        <v>7999</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1236" t="s">
+        <v>7974</v>
+      </c>
+      <c r="D1236" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1236" t="s">
+        <v>8000</v>
+      </c>
+      <c r="F1236" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1236" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1236" t="s">
+        <v>8001</v>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="s">
+        <v>8002</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1237" t="s">
+        <v>2826</v>
+      </c>
+      <c r="D1237" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1237" t="s">
+        <v>8000</v>
+      </c>
+      <c r="F1237" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1237" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1237" t="s">
+        <v>8003</v>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="s">
+        <v>8004</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>3651</v>
+      </c>
+      <c r="D1238" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1238" t="s">
+        <v>8005</v>
+      </c>
+      <c r="F1238" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1238" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1238" t="s">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="s">
+        <v>8007</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>5203</v>
+      </c>
+      <c r="D1239" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1239" t="s">
+        <v>8008</v>
+      </c>
+      <c r="F1239" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1239" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1239" t="s">
+        <v>8009</v>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="s">
+        <v>8010</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>3970</v>
+      </c>
+      <c r="D1240" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1240" t="s">
+        <v>8011</v>
+      </c>
+      <c r="F1240" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1240" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1240" t="s">
+        <v>8012</v>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="s">
+        <v>8013</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>7956</v>
+      </c>
+      <c r="D1241" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1241" t="s">
+        <v>8014</v>
+      </c>
+      <c r="F1241" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1241" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1241" t="s">
+        <v>8015</v>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="s">
+        <v>8016</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1242" t="s">
+        <v>7959</v>
+      </c>
+      <c r="D1242" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1242" t="s">
+        <v>8017</v>
+      </c>
+      <c r="F1242" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1242" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1242" t="s">
+        <v>8018</v>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="s">
+        <v>8019</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1243" t="s">
+        <v>7962</v>
+      </c>
+      <c r="D1243" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1243" t="s">
+        <v>8020</v>
+      </c>
+      <c r="F1243" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1243" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1243" t="s">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="s">
+        <v>8022</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1244" t="s">
+        <v>7966</v>
+      </c>
+      <c r="D1244" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1244" t="s">
+        <v>8023</v>
+      </c>
+      <c r="F1244" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1244" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1244" t="s">
+        <v>8024</v>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="s">
+        <v>8025</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>7970</v>
+      </c>
+      <c r="D1245" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1245" t="s">
+        <v>8023</v>
+      </c>
+      <c r="F1245" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1245" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1245" t="s">
+        <v>8026</v>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="s">
+        <v>8027</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1246" t="s">
+        <v>7974</v>
+      </c>
+      <c r="D1246" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1246" t="s">
+        <v>8023</v>
+      </c>
+      <c r="F1246" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1246" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1246" t="s">
+        <v>8028</v>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="s">
+        <v>8029</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1247" t="s">
+        <v>8030</v>
+      </c>
+      <c r="D1247" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1247" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1247" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1247" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1247" t="s">
+        <v>8031</v>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="s">
+        <v>8032</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1248" t="s">
+        <v>8033</v>
+      </c>
+      <c r="D1248" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1248" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1248" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1248" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1248" t="s">
+        <v>8034</v>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="s">
+        <v>8035</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1249" t="s">
+        <v>6120</v>
+      </c>
+      <c r="D1249" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1249" t="s">
+        <v>8036</v>
+      </c>
+      <c r="F1249" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1249" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1249" t="s">
+        <v>8037</v>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="s">
+        <v>8038</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1250" t="s">
+        <v>8039</v>
+      </c>
+      <c r="D1250" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1250" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1250" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1250" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1250" t="s">
+        <v>8040</v>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="s">
+        <v>8041</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1251" t="s">
+        <v>8042</v>
+      </c>
+      <c r="D1251" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1251" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1251" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1251" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1251" t="s">
+        <v>8043</v>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="s">
+        <v>8044</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1252" t="s">
+        <v>8045</v>
+      </c>
+      <c r="D1252" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1252" t="s">
+        <v>8036</v>
+      </c>
+      <c r="F1252" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1252" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1252" t="s">
+        <v>8046</v>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="s">
+        <v>8047</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1253" t="s">
+        <v>8048</v>
+      </c>
+      <c r="D1253" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1253" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1253" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1253" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1253" t="s">
+        <v>8049</v>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="s">
+        <v>8050</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1254" t="s">
+        <v>8051</v>
+      </c>
+      <c r="D1254" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1254" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1254" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1254" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1254" t="s">
+        <v>8052</v>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="s">
+        <v>8053</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1255" t="s">
+        <v>8054</v>
+      </c>
+      <c r="D1255" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1255" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1255" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1255" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1255" t="s">
+        <v>8055</v>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="s">
+        <v>8056</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1256" t="s">
+        <v>8057</v>
+      </c>
+      <c r="D1256" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1256" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1256" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1256" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1256" t="s">
+        <v>8058</v>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="s">
+        <v>8059</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1257" t="s">
+        <v>8030</v>
+      </c>
+      <c r="D1257" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1257" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1257" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1257" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1257" t="s">
+        <v>8060</v>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="s">
+        <v>8061</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1258" t="s">
+        <v>8033</v>
+      </c>
+      <c r="D1258" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1258" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1258" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1258" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1258" t="s">
+        <v>8062</v>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="s">
+        <v>8063</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1259" t="s">
+        <v>6120</v>
+      </c>
+      <c r="D1259" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1259" t="s">
+        <v>8036</v>
+      </c>
+      <c r="F1259" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1259" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1259" t="s">
+        <v>8064</v>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="s">
+        <v>8065</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1260" t="s">
+        <v>8039</v>
+      </c>
+      <c r="D1260" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1260" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1260" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1260" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1260" t="s">
+        <v>8066</v>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="s">
+        <v>8067</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1261" t="s">
+        <v>8042</v>
+      </c>
+      <c r="D1261" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1261" t="s">
+        <v>8068</v>
+      </c>
+      <c r="F1261" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1261" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1261" t="s">
+        <v>8069</v>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="s">
+        <v>8070</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1262" t="s">
+        <v>8045</v>
+      </c>
+      <c r="D1262" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1262" t="s">
+        <v>8036</v>
+      </c>
+      <c r="F1262" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1262" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1262" t="s">
+        <v>8071</v>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="s">
+        <v>8072</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1263" t="s">
+        <v>8048</v>
+      </c>
+      <c r="D1263" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1263" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1263" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1263" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1263" t="s">
+        <v>8073</v>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="s">
+        <v>8074</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1264" t="s">
+        <v>8051</v>
+      </c>
+      <c r="D1264" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1264" t="s">
+        <v>8068</v>
+      </c>
+      <c r="F1264" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1264" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1264" t="s">
+        <v>8075</v>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="s">
+        <v>8076</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1265" t="s">
+        <v>8054</v>
+      </c>
+      <c r="D1265" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1265" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1265" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1265" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1265" t="s">
+        <v>8077</v>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="s">
+        <v>8078</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1266" t="s">
+        <v>8057</v>
+      </c>
+      <c r="D1266" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1266" t="s">
+        <v>7949</v>
+      </c>
+      <c r="F1266" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1266" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1266" t="s">
+        <v>8079</v>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="s">
+        <v>8080</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1267" t="s">
+        <v>5925</v>
+      </c>
+      <c r="D1267" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1267" t="s">
+        <v>8082</v>
+      </c>
+      <c r="F1267" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1267" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1267" t="s">
+        <v>8083</v>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="s">
+        <v>8084</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1268" t="s">
+        <v>2656</v>
+      </c>
+      <c r="D1268" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1268" t="s">
+        <v>8086</v>
+      </c>
+      <c r="F1268" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1268" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1268" t="s">
+        <v>8087</v>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="s">
+        <v>8090</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1269" t="s">
+        <v>4204</v>
+      </c>
+      <c r="D1269" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1269" t="s">
+        <v>8092</v>
+      </c>
+      <c r="F1269" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1269" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1269" t="s">
+        <v>8093</v>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="s">
+        <v>8096</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1270" t="s">
+        <v>4210</v>
+      </c>
+      <c r="D1270" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1270" t="s">
+        <v>8098</v>
+      </c>
+      <c r="F1270" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1270" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1270" t="s">
+        <v>8099</v>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="s">
+        <v>8100</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1271" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D1271" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1271" t="s">
+        <v>8102</v>
+      </c>
+      <c r="F1271" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1271" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1271" t="s">
+        <v>8103</v>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="s">
+        <v>8104</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1272" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D1272" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1272" t="s">
+        <v>8106</v>
+      </c>
+      <c r="F1272" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1272" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1272" t="s">
+        <v>8107</v>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="s">
+        <v>8108</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1273" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D1273" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1273" t="s">
+        <v>8110</v>
+      </c>
+      <c r="F1273" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1273" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1273" t="s">
+        <v>8111</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="s">
+        <v>8112</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1274" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D1274" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1274" t="s">
+        <v>8114</v>
+      </c>
+      <c r="F1274" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1274" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1274" t="s">
+        <v>8115</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="s">
+        <v>8116</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1275" t="s">
+        <v>8118</v>
+      </c>
+      <c r="D1275" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1275" t="s">
+        <v>8119</v>
+      </c>
+      <c r="F1275" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G1275" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1275" t="s">
+        <v>8120</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="s">
+        <v>8121</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1276" t="s">
+        <v>8123</v>
+      </c>
+      <c r="D1276" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1276" t="s">
+        <v>8124</v>
+      </c>
+      <c r="F1276" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1276" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1276" t="s">
+        <v>8125</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="s">
+        <v>8126</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1277" t="s">
+        <v>8128</v>
+      </c>
+      <c r="D1277" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1277" t="s">
+        <v>8129</v>
+      </c>
+      <c r="F1277" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1277" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1277" t="s">
+        <v>8130</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="s">
+        <v>8131</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1278" t="s">
+        <v>8133</v>
+      </c>
+      <c r="D1278" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1278" t="s">
+        <v>8134</v>
+      </c>
+      <c r="F1278" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1278" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1278" t="s">
+        <v>8135</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="s">
+        <v>8136</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1279" t="s">
+        <v>8138</v>
+      </c>
+      <c r="D1279" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1279" t="s">
+        <v>8139</v>
+      </c>
+      <c r="F1279" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1279" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1279" t="s">
+        <v>8140</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="s">
+        <v>8141</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1280" t="s">
+        <v>8143</v>
+      </c>
+      <c r="D1280" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1280" t="s">
+        <v>8144</v>
+      </c>
+      <c r="F1280" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1280" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1280" t="s">
+        <v>8145</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="s">
+        <v>8146</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1281" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D1281" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1281" t="s">
+        <v>8148</v>
+      </c>
+      <c r="F1281" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1281" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1281" t="s">
+        <v>8149</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="s">
+        <v>8150</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1282" t="s">
+        <v>8152</v>
+      </c>
+      <c r="D1282" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1282" t="s">
+        <v>8153</v>
+      </c>
+      <c r="F1282" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1282" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1282" t="s">
+        <v>8154</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="s">
+        <v>8155</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>2149</v>
+      </c>
+      <c r="C1283" t="s">
+        <v>4796</v>
+      </c>
+      <c r="D1283" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1283" t="s">
+        <v>8157</v>
+      </c>
+      <c r="F1283" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G1283" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1283" t="s">
+        <v>8158</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="s">
+        <v>8159</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1284" t="s">
+        <v>8161</v>
+      </c>
+      <c r="D1284" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1284" t="s">
+        <v>8162</v>
+      </c>
+      <c r="F1284" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1284" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1284" t="s">
+        <v>8163</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="s">
+        <v>8164</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1285" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D1285" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1285" t="s">
+        <v>8166</v>
+      </c>
+      <c r="F1285" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1285" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1285" t="s">
+        <v>8167</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="s">
+        <v>8168</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1286" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D1286" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1286" t="s">
+        <v>8170</v>
+      </c>
+      <c r="F1286" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1286" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1286" t="s">
+        <v>8171</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="s">
+        <v>8174</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1287" t="s">
+        <v>2393</v>
+      </c>
+      <c r="D1287" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1287" t="s">
+        <v>8176</v>
+      </c>
+      <c r="F1287" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1287" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1287" t="s">
+        <v>8177</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="s">
+        <v>8180</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1288" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D1288" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1288" t="s">
+        <v>8182</v>
+      </c>
+      <c r="F1288" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1288" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1288" t="s">
+        <v>8183</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="s">
+        <v>8184</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1289" t="s">
+        <v>8186</v>
+      </c>
+      <c r="D1289" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1289" t="s">
+        <v>8187</v>
+      </c>
+      <c r="F1289" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G1289" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1289" t="s">
+        <v>8188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added showcase scenario 1
</commit_message>
<xml_diff>
--- a/src/main/java/resources/generateduuid.xlsx
+++ b/src/main/java/resources/generateduuid.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12940" uniqueCount="8196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13126" uniqueCount="8303">
   <si>
     <t>Vehicle uuid</t>
   </si>
@@ -24614,6 +24614,327 @@
   </si>
   <si>
     <t>2018-12-19T10:19:13.063</t>
+  </si>
+  <si>
+    <t>2018-12-26T10:20:06</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:09:59.405</t>
+  </si>
+  <si>
+    <t>ie14vu44104mh2c9xayuu7vv3fgi1hs549n</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:10:03.413</t>
+  </si>
+  <si>
+    <t>klhj0gk7mmw18r40h00f1r2b9joqcie2kk8</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:12:08.338</t>
+  </si>
+  <si>
+    <t>5UXUJ5C55KLJ62774</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:13:06</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:13:09.900</t>
+  </si>
+  <si>
+    <t>7cm325i77vp0z2ep05vawz63vw8txw10rai</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:13:13.476</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:09</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:12.373</t>
+  </si>
+  <si>
+    <t>dta7i6p7lo8h5dcffo7ri423hqz3x55kvme</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:15.799</t>
+  </si>
+  <si>
+    <t>a5db68bb0a0e0adf052ed355793a2935rty</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:20.347</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:21</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:28.545</t>
+  </si>
+  <si>
+    <t>8730rb46ju872hqhr37yy5fb589gt9xbr21</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:32.003</t>
+  </si>
+  <si>
+    <t>d4348fe40a0e0a17623e2bddc20b7fc2yv9</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:36.542</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:37</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:44.692</t>
+  </si>
+  <si>
+    <t>9pqz6vdnpt1l9tsgko6bknxf36d35p1v441</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:14:48.203</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:15:06</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:15:09.671</t>
+  </si>
+  <si>
+    <t>r7fwsdb030357sy7jy3n5n63raseu5j9op8</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:15:13.354</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:16:06</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:16:09.026</t>
+  </si>
+  <si>
+    <t>58631i0oq85970hndd417c0a2bu0zb2a97x</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:16:12.458</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:17:05</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:17:09.789</t>
+  </si>
+  <si>
+    <t>8ht5y7ra5ltey83juw7b63jzvmct10fbjcd</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:17:13.591</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:18:05</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:18:09.760</t>
+  </si>
+  <si>
+    <t>x8pb88lld00ufxt1x1fjlp1s782dxx85cfm</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:18:13.291</t>
+  </si>
+  <si>
+    <t>WBA2J1C57KVD10185</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:18:20</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:18:24.558</t>
+  </si>
+  <si>
+    <t>5495x14qt964cxymli7xh8ml05a7axnxyhh</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:18:28.340</t>
+  </si>
+  <si>
+    <t>WA19NAF46JA196444</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:18:55</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:19:00.263</t>
+  </si>
+  <si>
+    <t>m488gstreg5lcvf065lvony308u4x0f535z</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:19:03.735</t>
+  </si>
+  <si>
+    <t>WBXHU7C32J3F04299</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:19:30</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:19:37.910</t>
+  </si>
+  <si>
+    <t>ouw5e6w02671d0vq4rmhgsj1sp0516xc3w8</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:19:41.716</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:20:08</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:20:15.789</t>
+  </si>
+  <si>
+    <t>r5zmb0nzq41bqht05uq833e2m69u2hq72me</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:20:19.572</t>
+  </si>
+  <si>
+    <t>WBA8E5C50JA506607</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:20:47</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:20:54.042</t>
+  </si>
+  <si>
+    <t>5nfu2y521v152jg3mi7k3ya0r6e9j6zhw79</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:20:57.968</t>
+  </si>
+  <si>
+    <t>WUAPWAF58JA904537</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:21:24</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:21:31.342</t>
+  </si>
+  <si>
+    <t>rh3mj6qfjdlfxwye65b2yrr8t6dfm8332r1</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:21:35.176</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:22:05</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:08.806</t>
+  </si>
+  <si>
+    <t>128x0ec7l5dn1929gvg38e60b7p167pwq8r</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:12.264</t>
+  </si>
+  <si>
+    <t>WA1JCCFS0JR021654</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:18</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:25.499</t>
+  </si>
+  <si>
+    <t>k73gstyjw4tc915r9s4qdti8ls8a7q7pyb8</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:28.942</t>
+  </si>
+  <si>
+    <t>WBS3S7C50KAC09528</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:22:40</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:45.760</t>
+  </si>
+  <si>
+    <t>108qtdi6eeq2k5w3721840m6xik8e3hx2f4</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:22:49.568</t>
+  </si>
+  <si>
+    <t>WBY2Z6C57KVG97828</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:23:16</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:23:22.185</t>
+  </si>
+  <si>
+    <t>59o9ffs9v77ds7koj2983v46lh492f79zqy</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:23:25.632</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:24:06</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:24:12.090</t>
+  </si>
+  <si>
+    <t>f00nx70uqr2zdov2eos09g86r382faq928e</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:24:15.963</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:25:06</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:25:09.525</t>
+  </si>
+  <si>
+    <t>3w4s7u8r8gl02its8ndad1661hku4826708</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:25:13.305</t>
+  </si>
+  <si>
+    <t>3bd9dc580a0a00de6a568762d66fa01axnk</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:25:33.043</t>
+  </si>
+  <si>
+    <t>2018-12-26T15:26:05</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:26:10.273</t>
+  </si>
+  <si>
+    <t>rir6ddbqj2gscf8ps9182wta823j4e2gncu</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:26:14.011</t>
+  </si>
+  <si>
+    <t>04c16ffd0a0e0adf4d75c02155d62aed2fh</t>
+  </si>
+  <si>
+    <t>2018-12-19T15:26:34.529</t>
   </si>
 </sst>
 </file>
@@ -52355,6 +52676,222 @@
         <v>8195</v>
       </c>
     </row>
+    <row r="2610">
+      <c r="A2610" t="s">
+        <v>8198</v>
+      </c>
+      <c r="B2610" t="s">
+        <v>8199</v>
+      </c>
+    </row>
+    <row r="2611">
+      <c r="A2611" t="s">
+        <v>8200</v>
+      </c>
+      <c r="B2611" t="s">
+        <v>8201</v>
+      </c>
+    </row>
+    <row r="2612">
+      <c r="A2612" t="s">
+        <v>8205</v>
+      </c>
+      <c r="B2612" t="s">
+        <v>8206</v>
+      </c>
+    </row>
+    <row r="2613">
+      <c r="A2613" t="s">
+        <v>8209</v>
+      </c>
+      <c r="B2613" t="s">
+        <v>8210</v>
+      </c>
+    </row>
+    <row r="2614">
+      <c r="A2614" t="s">
+        <v>8211</v>
+      </c>
+      <c r="B2614" t="s">
+        <v>8212</v>
+      </c>
+    </row>
+    <row r="2615">
+      <c r="A2615" t="s">
+        <v>8215</v>
+      </c>
+      <c r="B2615" t="s">
+        <v>8216</v>
+      </c>
+    </row>
+    <row r="2616">
+      <c r="A2616" t="s">
+        <v>8217</v>
+      </c>
+      <c r="B2616" t="s">
+        <v>8218</v>
+      </c>
+    </row>
+    <row r="2617">
+      <c r="A2617" t="s">
+        <v>8221</v>
+      </c>
+      <c r="B2617" t="s">
+        <v>8222</v>
+      </c>
+    </row>
+    <row r="2618">
+      <c r="A2618" t="s">
+        <v>8225</v>
+      </c>
+      <c r="B2618" t="s">
+        <v>8226</v>
+      </c>
+    </row>
+    <row r="2619">
+      <c r="A2619" t="s">
+        <v>8229</v>
+      </c>
+      <c r="B2619" t="s">
+        <v>8230</v>
+      </c>
+    </row>
+    <row r="2620">
+      <c r="A2620" t="s">
+        <v>8233</v>
+      </c>
+      <c r="B2620" t="s">
+        <v>8234</v>
+      </c>
+    </row>
+    <row r="2621">
+      <c r="A2621" t="s">
+        <v>8237</v>
+      </c>
+      <c r="B2621" t="s">
+        <v>8238</v>
+      </c>
+    </row>
+    <row r="2622">
+      <c r="A2622" t="s">
+        <v>8242</v>
+      </c>
+      <c r="B2622" t="s">
+        <v>8243</v>
+      </c>
+    </row>
+    <row r="2623">
+      <c r="A2623" t="s">
+        <v>8247</v>
+      </c>
+      <c r="B2623" t="s">
+        <v>8248</v>
+      </c>
+    </row>
+    <row r="2624">
+      <c r="A2624" t="s">
+        <v>8252</v>
+      </c>
+      <c r="B2624" t="s">
+        <v>8253</v>
+      </c>
+    </row>
+    <row r="2625">
+      <c r="A2625" t="s">
+        <v>8256</v>
+      </c>
+      <c r="B2625" t="s">
+        <v>8257</v>
+      </c>
+    </row>
+    <row r="2626">
+      <c r="A2626" t="s">
+        <v>8261</v>
+      </c>
+      <c r="B2626" t="s">
+        <v>8262</v>
+      </c>
+    </row>
+    <row r="2627">
+      <c r="A2627" t="s">
+        <v>8266</v>
+      </c>
+      <c r="B2627" t="s">
+        <v>8267</v>
+      </c>
+    </row>
+    <row r="2628">
+      <c r="A2628" t="s">
+        <v>8270</v>
+      </c>
+      <c r="B2628" t="s">
+        <v>8271</v>
+      </c>
+    </row>
+    <row r="2629">
+      <c r="A2629" t="s">
+        <v>8275</v>
+      </c>
+      <c r="B2629" t="s">
+        <v>8276</v>
+      </c>
+    </row>
+    <row r="2630">
+      <c r="A2630" t="s">
+        <v>8280</v>
+      </c>
+      <c r="B2630" t="s">
+        <v>8281</v>
+      </c>
+    </row>
+    <row r="2631">
+      <c r="A2631" t="s">
+        <v>8285</v>
+      </c>
+      <c r="B2631" t="s">
+        <v>8286</v>
+      </c>
+    </row>
+    <row r="2632">
+      <c r="A2632" t="s">
+        <v>8289</v>
+      </c>
+      <c r="B2632" t="s">
+        <v>8290</v>
+      </c>
+    </row>
+    <row r="2633">
+      <c r="A2633" t="s">
+        <v>8293</v>
+      </c>
+      <c r="B2633" t="s">
+        <v>8294</v>
+      </c>
+    </row>
+    <row r="2634">
+      <c r="A2634" t="s">
+        <v>8295</v>
+      </c>
+      <c r="B2634" t="s">
+        <v>8296</v>
+      </c>
+    </row>
+    <row r="2635">
+      <c r="A2635" t="s">
+        <v>8299</v>
+      </c>
+      <c r="B2635" t="s">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="2636">
+      <c r="A2636" t="s">
+        <v>8301</v>
+      </c>
+      <c r="B2636" t="s">
+        <v>8302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -87928,6 +88465,578 @@
         <v>8193</v>
       </c>
     </row>
+    <row r="1291">
+      <c r="A1291" t="s">
+        <v>8194</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1291" t="s">
+        <v>5442</v>
+      </c>
+      <c r="D1291" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1291" t="s">
+        <v>8196</v>
+      </c>
+      <c r="F1291" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1291" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1291" t="s">
+        <v>8197</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="s">
+        <v>8200</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1292" t="s">
+        <v>8202</v>
+      </c>
+      <c r="D1292" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1292" t="s">
+        <v>8203</v>
+      </c>
+      <c r="F1292" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1292" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1292" t="s">
+        <v>8204</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="s">
+        <v>8205</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1293" t="s">
+        <v>3146</v>
+      </c>
+      <c r="D1293" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1293" t="s">
+        <v>8207</v>
+      </c>
+      <c r="F1293" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G1293" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1293" t="s">
+        <v>8208</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="s">
+        <v>8211</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1294" t="s">
+        <v>4204</v>
+      </c>
+      <c r="D1294" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1294" t="s">
+        <v>8213</v>
+      </c>
+      <c r="F1294" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1294" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1294" t="s">
+        <v>8214</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="s">
+        <v>8217</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1295" t="s">
+        <v>4210</v>
+      </c>
+      <c r="D1295" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1295" t="s">
+        <v>8219</v>
+      </c>
+      <c r="F1295" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1295" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1295" t="s">
+        <v>8220</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="s">
+        <v>8221</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1296" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D1296" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1296" t="s">
+        <v>8223</v>
+      </c>
+      <c r="F1296" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1296" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1296" t="s">
+        <v>8224</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="s">
+        <v>8225</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1297" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D1297" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1297" t="s">
+        <v>8227</v>
+      </c>
+      <c r="F1297" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1297" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1297" t="s">
+        <v>8228</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="s">
+        <v>8229</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1298" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D1298" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1298" t="s">
+        <v>8231</v>
+      </c>
+      <c r="F1298" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1298" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1298" t="s">
+        <v>8232</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="s">
+        <v>8233</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1299" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D1299" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1299" t="s">
+        <v>8235</v>
+      </c>
+      <c r="F1299" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1299" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1299" t="s">
+        <v>8236</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="s">
+        <v>8237</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1300" t="s">
+        <v>8239</v>
+      </c>
+      <c r="D1300" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1300" t="s">
+        <v>8240</v>
+      </c>
+      <c r="F1300" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G1300" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1300" t="s">
+        <v>8241</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="s">
+        <v>8242</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1301" t="s">
+        <v>8244</v>
+      </c>
+      <c r="D1301" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1301" t="s">
+        <v>8245</v>
+      </c>
+      <c r="F1301" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1301" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1301" t="s">
+        <v>8246</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="s">
+        <v>8247</v>
+      </c>
+      <c r="B1302" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1302" t="s">
+        <v>8249</v>
+      </c>
+      <c r="D1302" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1302" t="s">
+        <v>8250</v>
+      </c>
+      <c r="F1302" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1302" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1302" t="s">
+        <v>8251</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="s">
+        <v>8252</v>
+      </c>
+      <c r="B1303" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1303" t="s">
+        <v>6045</v>
+      </c>
+      <c r="D1303" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1303" t="s">
+        <v>8254</v>
+      </c>
+      <c r="F1303" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1303" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1303" t="s">
+        <v>8255</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="s">
+        <v>8256</v>
+      </c>
+      <c r="B1304" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1304" t="s">
+        <v>8258</v>
+      </c>
+      <c r="D1304" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1304" t="s">
+        <v>8259</v>
+      </c>
+      <c r="F1304" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1304" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1304" t="s">
+        <v>8260</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="s">
+        <v>8261</v>
+      </c>
+      <c r="B1305" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1305" t="s">
+        <v>8263</v>
+      </c>
+      <c r="D1305" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1305" t="s">
+        <v>8264</v>
+      </c>
+      <c r="F1305" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1305" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1305" t="s">
+        <v>8265</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="s">
+        <v>8266</v>
+      </c>
+      <c r="B1306" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1306" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D1306" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1306" t="s">
+        <v>8268</v>
+      </c>
+      <c r="F1306" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1306" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1306" t="s">
+        <v>8269</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="s">
+        <v>8270</v>
+      </c>
+      <c r="B1307" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1307" t="s">
+        <v>8272</v>
+      </c>
+      <c r="D1307" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1307" t="s">
+        <v>8273</v>
+      </c>
+      <c r="F1307" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1307" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1307" t="s">
+        <v>8274</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="s">
+        <v>8275</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>2149</v>
+      </c>
+      <c r="C1308" t="s">
+        <v>8277</v>
+      </c>
+      <c r="D1308" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1308" t="s">
+        <v>8278</v>
+      </c>
+      <c r="F1308" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G1308" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1308" t="s">
+        <v>8279</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="s">
+        <v>8280</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1309" t="s">
+        <v>8282</v>
+      </c>
+      <c r="D1309" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1309" t="s">
+        <v>8283</v>
+      </c>
+      <c r="F1309" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G1309" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1309" t="s">
+        <v>8284</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="s">
+        <v>8285</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1310" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D1310" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1310" t="s">
+        <v>8287</v>
+      </c>
+      <c r="F1310" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1310" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1310" t="s">
+        <v>8288</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="s">
+        <v>8289</v>
+      </c>
+      <c r="B1311" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1311" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D1311" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E1311" t="s">
+        <v>8291</v>
+      </c>
+      <c r="F1311" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1311" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1311" t="s">
+        <v>8292</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="s">
+        <v>8295</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1312" t="s">
+        <v>2393</v>
+      </c>
+      <c r="D1312" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E1312" t="s">
+        <v>8297</v>
+      </c>
+      <c r="F1312" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G1312" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1312" t="s">
+        <v>8298</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>